<commit_message>
Use production-centric rules always for Power Gen
The OECM scope rules for Power (aka Electricity) Utilities are just so different from corp disclosures that we really need to use production-centric rules for both PC and S3 cases.  And we need to let all-zero data (such as S3 data for Production-Centric Power Utilities) appear as zeros in the data, not the absence of data in the benchmark.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/notebooks/benchmark_OECM_PC.xlsx
+++ b/notebooks/benchmark_OECM_PC.xlsx
@@ -8368,100 +8368,100 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.3814070550303191</v>
+        <v>1.408690537419691</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3640981452944985</v>
+        <v>1.298366199526652</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3475747437245375</v>
+        <v>1.196682126623134</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3318012026055859</v>
+        <v>1.10296163956005</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3167434919775529</v>
+        <v>1.016581054631317</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3023691262186074</v>
+        <v>0.9369655331327201</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2886470939604449</v>
+        <v>0.8635852559706334</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2588896253744872</v>
+        <v>0.7622209822801315</v>
       </c>
       <c r="M2" t="n">
-        <v>0.232199940789035</v>
+        <v>0.6727544522226592</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2082617734273438</v>
+        <v>0.5937891549921559</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1867914613746983</v>
+        <v>0.5240924967815813</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1675345862483392</v>
+        <v>0.462576560844026</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.144358759441082</v>
+        <v>0.415387259844895</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1243889509266912</v>
+        <v>0.3730119298016711</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1071816575076465</v>
+        <v>0.3349594781176503</v>
       </c>
       <c r="T2" t="n">
-        <v>0.09235472781547018</v>
+        <v>0.300788910532979</v>
       </c>
       <c r="U2" t="n">
-        <v>0.07957887523115678</v>
+        <v>0.2701042203912157</v>
       </c>
       <c r="V2" t="n">
-        <v>0.07491716049156599</v>
+        <v>0.2471192383916059</v>
       </c>
       <c r="W2" t="n">
-        <v>0.07052852807753199</v>
+        <v>0.2260902028661281</v>
       </c>
       <c r="X2" t="n">
-        <v>0.06639698088054487</v>
+        <v>0.2068506691941282</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.0625074588995408</v>
+        <v>0.1892483566454832</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.05884578434533363</v>
+        <v>0.1731439430800384</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.05215959422985029</v>
+        <v>0.160228088209161</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.04562789532346201</v>
+        <v>0.1482757051414436</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.0392479119090937</v>
+        <v>0.1372149226825468</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.03301691301862297</v>
+        <v>0.1269792309456017</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.02693221175394886</v>
+        <v>0.1175070814188298</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.02129785636090432</v>
+        <v>0.1065579160137834</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.01578959691861381</v>
+        <v>0.0966289803822923</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.010405277586108</v>
+        <v>0.08762521076813901</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.005142775439520216</v>
+        <v>0.07946040133905673</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0</v>
+        <v>0.07205637881626364</v>
       </c>
     </row>
     <row r="3">
@@ -8474,100 +8474,100 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.4761262643242212</v>
+        <v>1.503409746713593</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4524439041972547</v>
+        <v>1.386632472655432</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4299394966916991</v>
+        <v>1.278925867299708</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4085544508406556</v>
+        <v>1.179585366925674</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3882330899721972</v>
+        <v>1.087961134763024</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3689225067533188</v>
+        <v>1.003453810078869</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3505724254439503</v>
+        <v>0.9255105874541389</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3127174783752844</v>
+        <v>0.8159821394366535</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2789501232378915</v>
+        <v>0.7194157051311004</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2488289802626677</v>
+        <v>0.6342773104649035</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2219603300399211</v>
+        <v>0.559214517699858</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1979929671351961</v>
+        <v>0.4930349417308829</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1724380961380849</v>
+        <v>0.4433056318981519</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1501815818509527</v>
+        <v>0.3985922023755626</v>
       </c>
       <c r="S3" t="n">
-        <v>0.130797706727133</v>
+        <v>0.3583887331057021</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1139157004089617</v>
+        <v>0.3222403329809468</v>
       </c>
       <c r="U3" t="n">
-        <v>0.09921264771664677</v>
+        <v>0.2897379928767057</v>
       </c>
       <c r="V3" t="n">
-        <v>0.09158103950678134</v>
+        <v>0.2636565716701991</v>
       </c>
       <c r="W3" t="n">
-        <v>0.08453646778076451</v>
+        <v>0.2399229286249111</v>
       </c>
       <c r="X3" t="n">
-        <v>0.07803377667840362</v>
+        <v>0.2183257231758221</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.07203128380625962</v>
+        <v>0.1986726390572099</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.06649051305258523</v>
+        <v>0.1807886717872899</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.05862569513807737</v>
+        <v>0.1664303177763133</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.0509430085277204</v>
+        <v>0.1532123135885109</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.0434391782759191</v>
+        <v>0.1410440918985318</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.03611098225615166</v>
+        <v>0.1298422782969663</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.02895525035939728</v>
+        <v>0.1195301200242782</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.0228976650221847</v>
+        <v>0.1080230340217404</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.01697564745254894</v>
+        <v>0.09762372761687142</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.01118687987148351</v>
+        <v>0.08822555559673544</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.00552907988968391</v>
+        <v>0.07973213941287223</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1.665685719782396e-18</v>
+        <v>0.07205637881626359</v>
       </c>
     </row>
     <row r="4">
@@ -8694,100 +8694,100 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.8178538601825653</v>
+        <v>2.704884724080175</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7554057448650418</v>
+        <v>2.477856248639105</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6977259228778694</v>
+        <v>2.269882902683682</v>
       </c>
       <c r="H5" t="n">
-        <v>0.644450306030898</v>
+        <v>2.079365336356981</v>
       </c>
       <c r="I5" t="n">
-        <v>0.595242606481192</v>
+        <v>1.904838437670506</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5497922140074765</v>
+        <v>1.744960065547663</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5078122353675866</v>
+        <v>1.598500728534122</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4587908942121944</v>
+        <v>1.429530470980587</v>
       </c>
       <c r="M5" t="n">
-        <v>0.414501798011345</v>
+        <v>1.278421292517012</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3744881224150309</v>
+        <v>1.143285179531555</v>
       </c>
       <c r="O5" t="n">
-        <v>0.3383371423303134</v>
+        <v>1.022433691762925</v>
       </c>
       <c r="P5" t="n">
-        <v>0.3056759748267203</v>
+        <v>0.9143568663072242</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.281770022825228</v>
+        <v>0.8467830670397301</v>
       </c>
       <c r="R5" t="n">
-        <v>0.2597336797827701</v>
+        <v>0.7842031804508653</v>
       </c>
       <c r="S5" t="n">
-        <v>0.2394207294909531</v>
+        <v>0.7262481409543803</v>
       </c>
       <c r="T5" t="n">
-        <v>0.2206963908489726</v>
+        <v>0.6725761580518614</v>
       </c>
       <c r="U5" t="n">
-        <v>0.2034364235599865</v>
+        <v>0.622870700619415</v>
       </c>
       <c r="V5" t="n">
-        <v>0.1774778392160342</v>
+        <v>0.566568532227381</v>
       </c>
       <c r="W5" t="n">
-        <v>0.1548315825730425</v>
+        <v>0.5153555969016843</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1350749990419483</v>
+        <v>0.4687718716282349</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.1178393649601498</v>
+        <v>0.4263989155273694</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.1028030059796556</v>
+        <v>0.3878561111855876</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.08842812740109338</v>
+        <v>0.3640727444478852</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.07606327890073039</v>
+        <v>0.3417477755981289</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.06542739925824508</v>
+        <v>0.320791775565026</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.05627872786400091</v>
+        <v>0.3011207990748527</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.04840930933978908</v>
+        <v>0.2826560483845628</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.03779513571979451</v>
+        <v>0.2619643661546017</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.02766395109921778</v>
+        <v>0.2427874072640229</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.01799865219796534</v>
+        <v>0.2250142872149219</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.008782679301163238</v>
+        <v>0.2085422387487315</v>
       </c>
       <c r="AJ5" t="n">
-        <v>-2.014003882331952e-18</v>
+        <v>0.1932760176281326</v>
       </c>
     </row>
     <row r="6">
@@ -8800,100 +8800,100 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1.121311439369287</v>
+        <v>3.008342303266898</v>
       </c>
       <c r="F6" t="n">
-        <v>1.028218628020623</v>
+        <v>2.750516446650601</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9428545093620755</v>
+        <v>2.514787201935064</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8645774367419551</v>
+        <v>2.299260809262758</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7927990338923395</v>
+        <v>2.102205810870889</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7269797723488594</v>
+        <v>1.922039141212666</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6666249160391494</v>
+        <v>1.757313409205685</v>
       </c>
       <c r="L6" t="n">
-        <v>0.594710048472054</v>
+        <v>1.565310710553145</v>
       </c>
       <c r="M6" t="n">
-        <v>0.5305532890295718</v>
+        <v>1.394286077678023</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4733177003201815</v>
+        <v>1.241947463401557</v>
       </c>
       <c r="O6" t="n">
-        <v>0.4222566329692441</v>
+        <v>1.106253247840111</v>
       </c>
       <c r="P6" t="n">
-        <v>0.3767039854328483</v>
+        <v>0.9853848769133524</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.3412238771933587</v>
+        <v>0.9064714175803337</v>
       </c>
       <c r="R6" t="n">
-        <v>0.309085485870507</v>
+        <v>0.8338776554639097</v>
       </c>
       <c r="S6" t="n">
-        <v>0.2799740696975669</v>
+        <v>0.7670974845937303</v>
       </c>
       <c r="T6" t="n">
-        <v>0.2536045310644514</v>
+        <v>0.7056653299369957</v>
       </c>
       <c r="U6" t="n">
-        <v>0.2297186244636684</v>
+        <v>0.6491529015230969</v>
       </c>
       <c r="V6" t="n">
-        <v>0.1997435215140175</v>
+        <v>0.5890094490173027</v>
       </c>
       <c r="W6" t="n">
-        <v>0.1736797548739059</v>
+        <v>0.5344382351487073</v>
       </c>
       <c r="X6" t="n">
-        <v>0.1510169492578169</v>
+        <v>0.4849229968473298</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.1313113262953165</v>
+        <v>0.4399953023682239</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.1141770145548254</v>
+        <v>0.3992301197607573</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.09747598618568049</v>
+        <v>0.3734740053503278</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.08321786937517552</v>
+        <v>0.3493795326765505</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.07104533182308148</v>
+        <v>0.3268395018249901</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.06065330934028263</v>
+        <v>0.3057536288254858</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.05178136042898777</v>
+        <v>0.2860280994737616</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.04042783447770868</v>
+        <v>0.26446155917292</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.02959094112877773</v>
+        <v>0.2445211376394427</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.01925238573756725</v>
+        <v>0.2260842253954679</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.009394455087834675</v>
+        <v>0.2090374577270235</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0</v>
+        <v>0.1932760176281326</v>
       </c>
     </row>
     <row r="7">
@@ -9020,100 +9020,100 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1.410439505993448</v>
+        <v>6.152219207315672</v>
       </c>
       <c r="F8" t="n">
-        <v>1.321502559276045</v>
+        <v>5.630505215030543</v>
       </c>
       <c r="G8" t="n">
-        <v>1.238173637899541</v>
+        <v>5.153033061433872</v>
       </c>
       <c r="H8" t="n">
-        <v>1.160099121131662</v>
+        <v>4.716050996870713</v>
       </c>
       <c r="I8" t="n">
-        <v>1.086947686217536</v>
+        <v>4.316125423595959</v>
       </c>
       <c r="J8" t="n">
-        <v>1.018408902354103</v>
+        <v>3.950113916192262</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9541919133231563</v>
+        <v>3.615140529881977</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8312369107529264</v>
+        <v>3.163346353091571</v>
       </c>
       <c r="M8" t="n">
-        <v>0.7241256105301562</v>
+        <v>2.768014152397121</v>
       </c>
       <c r="N8" t="n">
-        <v>0.6308164291582206</v>
+        <v>2.422087717452342</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5495308569525542</v>
+        <v>2.119392672162841</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4787195589467842</v>
+        <v>1.854526269404581</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4490754527244681</v>
+        <v>1.711511825606773</v>
       </c>
       <c r="R8" t="n">
-        <v>0.4212670204730534</v>
+        <v>1.579526145042048</v>
       </c>
       <c r="S8" t="n">
-        <v>0.3951805903920756</v>
+        <v>1.457718728871119</v>
       </c>
       <c r="T8" t="n">
-        <v>0.3707095296642591</v>
+        <v>1.345304665688243</v>
       </c>
       <c r="U8" t="n">
-        <v>0.3477538085753413</v>
+        <v>1.241559573652544</v>
       </c>
       <c r="V8" t="n">
-        <v>0.3000326536849125</v>
+        <v>1.097144631325459</v>
       </c>
       <c r="W8" t="n">
-        <v>0.2540412283532387</v>
+        <v>0.9695276550484294</v>
       </c>
       <c r="X8" t="n">
-        <v>0.2097302027446903</v>
+        <v>0.8567547496159306</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.1670515134766774</v>
+        <v>0.7570992917708881</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.1259583329794234</v>
+        <v>0.6690354945297197</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1109407711418166</v>
+        <v>0.62823296982127</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.09648766744330112</v>
+        <v>0.5899188721636958</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.08258215578396305</v>
+        <v>0.5539414396444249</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.06920782507007936</v>
+        <v>0.5201581658675778</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.05634870763222379</v>
+        <v>0.488435235486982</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.04423833099591382</v>
+        <v>0.4556733397868228</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.03256002907284639</v>
+        <v>0.4251089551011956</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.02130189853927609</v>
+        <v>0.3965946829186348</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.01045232976517911</v>
+        <v>0.3699930115136971</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0</v>
+        <v>0.3451756527887191</v>
       </c>
     </row>
     <row r="9">
@@ -9126,100 +9126,100 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1.541411682955603</v>
+        <v>6.283191384277828</v>
       </c>
       <c r="F9" t="n">
-        <v>1.438698065502921</v>
+        <v>5.74724263109073</v>
       </c>
       <c r="G9" t="n">
-        <v>1.342828879895978</v>
+        <v>5.257009669207008</v>
       </c>
       <c r="H9" t="n">
-        <v>1.253348040092311</v>
+        <v>4.808592995993124</v>
       </c>
       <c r="I9" t="n">
-        <v>1.169829851831104</v>
+        <v>4.398425731752941</v>
       </c>
       <c r="J9" t="n">
-        <v>1.091876987444277</v>
+        <v>4.023245247386719</v>
       </c>
       <c r="K9" t="n">
-        <v>1.019118595618224</v>
+        <v>3.680067212177044</v>
       </c>
       <c r="L9" t="n">
-        <v>0.8807241409824588</v>
+        <v>3.21303901454048</v>
       </c>
       <c r="M9" t="n">
-        <v>0.761123401971431</v>
+        <v>2.805280206513414</v>
       </c>
       <c r="N9" t="n">
-        <v>0.6577642261313947</v>
+        <v>2.449269056940296</v>
       </c>
       <c r="O9" t="n">
-        <v>0.5684410386772899</v>
+        <v>2.138438398900999</v>
       </c>
       <c r="P9" t="n">
-        <v>0.4912477778746952</v>
+        <v>1.867054488332492</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.461186879546032</v>
+        <v>1.723654059984332</v>
       </c>
       <c r="R9" t="n">
-        <v>0.4329654961200842</v>
+        <v>1.591267602025864</v>
       </c>
       <c r="S9" t="n">
-        <v>0.4064710622622991</v>
+        <v>1.469049178743072</v>
       </c>
       <c r="T9" t="n">
-        <v>0.3815979008424679</v>
+        <v>1.356217827107257</v>
       </c>
       <c r="U9" t="n">
-        <v>0.3582468014252147</v>
+        <v>1.252052566502417</v>
       </c>
       <c r="V9" t="n">
-        <v>0.3090006223543075</v>
+        <v>1.105679163336098</v>
       </c>
       <c r="W9" t="n">
-        <v>0.2615396858491244</v>
+        <v>0.9764177998138814</v>
       </c>
       <c r="X9" t="n">
-        <v>0.2158130764298169</v>
+        <v>0.8622679629023403</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.171771185811172</v>
+        <v>0.7614630130559624</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.1293656812762039</v>
+        <v>0.6724428428265</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.1140138927394435</v>
+        <v>0.6312698832223207</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.09923886924360061</v>
+        <v>0.5926179001154772</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.08502337983229304</v>
+        <v>0.5563325367980426</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.07135065835755454</v>
+        <v>0.5222688876590383</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.05820439164906948</v>
+        <v>0.4902909195038275</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.0460049223787873</v>
+        <v>0.4574375276531319</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.03424020531656122</v>
+        <v>0.4267855744038031</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.02289826826046104</v>
+        <v>0.3981875458571967</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.01196743434006788</v>
+        <v>0.3715058127193443</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.00143631516509012</v>
+        <v>0.3466119679538092</v>
       </c>
     </row>
     <row r="10">
@@ -16226,100 +16226,100 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.3548824300649865</v>
+        <v>1.346173498472834</v>
       </c>
       <c r="F74" t="n">
-        <v>0.3385805375006509</v>
+        <v>1.240036070043543</v>
       </c>
       <c r="G74" t="n">
-        <v>0.3230274892821187</v>
+        <v>1.14226691934841</v>
       </c>
       <c r="H74" t="n">
-        <v>0.3081888864675475</v>
+        <v>1.052206259606537</v>
       </c>
       <c r="I74" t="n">
-        <v>0.2940319102661723</v>
+        <v>0.9692463241312552</v>
       </c>
       <c r="J74" t="n">
-        <v>0.2805252494524268</v>
+        <v>0.8928272648684346</v>
       </c>
       <c r="K74" t="n">
-        <v>0.2676390311143719</v>
+        <v>0.8224333743096054</v>
       </c>
       <c r="L74" t="n">
-        <v>0.2400110584805717</v>
+        <v>0.7256998250581227</v>
       </c>
       <c r="M74" t="n">
-        <v>0.2152350797008661</v>
+        <v>0.6403439506956778</v>
       </c>
       <c r="N74" t="n">
-        <v>0.1930166877606107</v>
+        <v>0.565027523824617</v>
       </c>
       <c r="O74" t="n">
-        <v>0.1730918668362737</v>
+        <v>0.4985697176221219</v>
       </c>
       <c r="P74" t="n">
-        <v>0.1552238550587152</v>
+        <v>0.4399285925882761</v>
       </c>
       <c r="Q74" t="n">
-        <v>0.1337303581531739</v>
+        <v>0.3952477489766926</v>
       </c>
       <c r="R74" t="n">
-        <v>0.1152130172582778</v>
+        <v>0.3551048640690371</v>
       </c>
       <c r="S74" t="n">
-        <v>0.09925973076773048</v>
+        <v>0.3190390452873276</v>
       </c>
       <c r="T74" t="n">
-        <v>0.08551545985464123</v>
+        <v>0.2866362100803579</v>
       </c>
       <c r="U74" t="n">
-        <v>0.07367432711723809</v>
+        <v>0.2575243317169447</v>
       </c>
       <c r="V74" t="n">
-        <v>0.06934754010591407</v>
+        <v>0.2355099217515145</v>
       </c>
       <c r="W74" t="n">
-        <v>0.06527485905760171</v>
+        <v>0.2153774087039208</v>
       </c>
       <c r="X74" t="n">
-        <v>0.06144136069545168</v>
+        <v>0.1969659190365615</v>
       </c>
       <c r="Y74" t="n">
-        <v>0.05783299816514832</v>
+        <v>0.1801283314502569</v>
       </c>
       <c r="Z74" t="n">
-        <v>0.0544365495638778</v>
+        <v>0.1647301012772207</v>
       </c>
       <c r="AA74" t="n">
-        <v>0.04824711948094131</v>
+        <v>0.1525776329927764</v>
       </c>
       <c r="AB74" t="n">
-        <v>0.04220070800779809</v>
+        <v>0.141321676543506</v>
       </c>
       <c r="AC74" t="n">
-        <v>0.03629474551782428</v>
+        <v>0.1308960944623704</v>
       </c>
       <c r="AD74" t="n">
-        <v>0.03052670381114119</v>
+        <v>0.1212396283752488</v>
       </c>
       <c r="AE74" t="n">
-        <v>0.02489409548608594</v>
+        <v>0.1122955390605186</v>
       </c>
       <c r="AF74" t="n">
-        <v>0.01968612436071304</v>
+        <v>0.1020297136028341</v>
       </c>
       <c r="AG74" t="n">
-        <v>0.01459470677602807</v>
+        <v>0.09270236863341588</v>
       </c>
       <c r="AH74" t="n">
-        <v>0.009617850036019518</v>
+        <v>0.08422771021094999</v>
       </c>
       <c r="AI74" t="n">
-        <v>0.004753591870750925</v>
+        <v>0.07652778749843643</v>
       </c>
       <c r="AJ74" t="n">
-        <v>0</v>
+        <v>0.06953177576284711</v>
       </c>
     </row>
     <row r="75">
@@ -16332,100 +16332,100 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.4656595472948267</v>
+        <v>1.456950615702674</v>
       </c>
       <c r="F75" t="n">
-        <v>0.4418927939710958</v>
+        <v>1.343268922138375</v>
       </c>
       <c r="G75" t="n">
-        <v>0.4193390697086877</v>
+        <v>1.238457486297543</v>
       </c>
       <c r="H75" t="n">
-        <v>0.3979364628327695</v>
+        <v>1.141824187315211</v>
       </c>
       <c r="I75" t="n">
-        <v>0.3776262215725887</v>
+        <v>1.052730908539891</v>
       </c>
       <c r="J75" t="n">
-        <v>0.3583525927834297</v>
+        <v>0.9705893237391052</v>
       </c>
       <c r="K75" t="n">
-        <v>0.3400626689000247</v>
+        <v>0.8948570120952585</v>
       </c>
       <c r="L75" t="n">
-        <v>0.3029589120863751</v>
+        <v>0.7885736652403812</v>
       </c>
       <c r="M75" t="n">
-        <v>0.2699034936985208</v>
+        <v>0.6949137315855912</v>
       </c>
       <c r="N75" t="n">
-        <v>0.2404547052568572</v>
+        <v>0.6123779117059496</v>
       </c>
       <c r="O75" t="n">
-        <v>0.2142190324692301</v>
+        <v>0.5396449799454724</v>
       </c>
       <c r="P75" t="n">
-        <v>0.1908458968313094</v>
+        <v>0.4755506343608703</v>
       </c>
       <c r="Q75" t="n">
-        <v>0.1665615031864699</v>
+        <v>0.427897601015277</v>
       </c>
       <c r="R75" t="n">
-        <v>0.1453672036148543</v>
+        <v>0.3850196881783297</v>
       </c>
       <c r="S75" t="n">
-        <v>0.126869795736324</v>
+        <v>0.3464384000592836</v>
       </c>
       <c r="T75" t="n">
-        <v>0.1107261106351213</v>
+        <v>0.3117231890231201</v>
       </c>
       <c r="U75" t="n">
-        <v>0.0966366462972944</v>
+        <v>0.280486650897001</v>
       </c>
       <c r="V75" t="n">
-        <v>0.08881784451931178</v>
+        <v>0.2548444296893259</v>
       </c>
       <c r="W75" t="n">
-        <v>0.0816316563882816</v>
+        <v>0.2315464323738058</v>
       </c>
       <c r="X75" t="n">
-        <v>0.07502689758751771</v>
+        <v>0.2103783489024915</v>
       </c>
       <c r="Y75" t="n">
-        <v>0.06895652508670559</v>
+        <v>0.1911454615525544</v>
       </c>
       <c r="Z75" t="n">
-        <v>0.06337730207339069</v>
+        <v>0.1736708537867336</v>
       </c>
       <c r="AA75" t="n">
-        <v>0.05580942942493658</v>
+        <v>0.1598325067166176</v>
       </c>
       <c r="AB75" t="n">
-        <v>0.04841690135344828</v>
+        <v>0.1470968193355484</v>
       </c>
       <c r="AC75" t="n">
-        <v>0.04119656436872544</v>
+        <v>0.1353759301103757</v>
       </c>
       <c r="AD75" t="n">
-        <v>0.03414531584557488</v>
+        <v>0.1245889784431279</v>
       </c>
       <c r="AE75" t="n">
-        <v>0.02726010325184839</v>
+        <v>0.114661546826281</v>
       </c>
       <c r="AF75" t="n">
-        <v>0.02155715129323389</v>
+        <v>0.1037458901185651</v>
       </c>
       <c r="AG75" t="n">
-        <v>0.01598183046527434</v>
+        <v>0.09386939226278071</v>
       </c>
       <c r="AH75" t="n">
-        <v>0.0105319586802914</v>
+        <v>0.08493312644687606</v>
       </c>
       <c r="AI75" t="n">
-        <v>0.005205387168465126</v>
+        <v>0.07684758358557363</v>
       </c>
       <c r="AJ75" t="n">
-        <v>-1.607325928140386e-18</v>
+        <v>0.0695317757628471</v>
       </c>
     </row>
     <row r="76">
@@ -16552,100 +16552,100 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.1866788585238317</v>
+        <v>0.7007776553081582</v>
       </c>
       <c r="F77" t="n">
-        <v>0.172454068596472</v>
+        <v>0.641710209559712</v>
       </c>
       <c r="G77" t="n">
-        <v>0.1593131970628585</v>
+        <v>0.5876214658586527</v>
       </c>
       <c r="H77" t="n">
-        <v>0.147173650149002</v>
+        <v>0.5380917772444155</v>
       </c>
       <c r="I77" t="n">
-        <v>0.1359591276649522</v>
+        <v>0.4927368681383411</v>
       </c>
       <c r="J77" t="n">
-        <v>0.125599143438382</v>
+        <v>0.451204852945559</v>
       </c>
       <c r="K77" t="n">
-        <v>0.1160285822907777</v>
+        <v>0.4131735059542259</v>
       </c>
       <c r="L77" t="n">
-        <v>0.1048278346125823</v>
+        <v>0.3692896447580772</v>
       </c>
       <c r="M77" t="n">
-        <v>0.09470834420801449</v>
+        <v>0.3300667631400727</v>
       </c>
       <c r="N77" t="n">
-        <v>0.08556573257258845</v>
+        <v>0.2950098105272743</v>
       </c>
       <c r="O77" t="n">
-        <v>0.07730569731641618</v>
+        <v>0.2636763165105614</v>
       </c>
       <c r="P77" t="n">
-        <v>0.06984303947269496</v>
+        <v>0.2356708062159513</v>
       </c>
       <c r="Q77" t="n">
-        <v>0.06438083607179283</v>
+        <v>0.2183112596134211</v>
       </c>
       <c r="R77" t="n">
-        <v>0.05934581433735428</v>
+        <v>0.2022304197929659</v>
       </c>
       <c r="S77" t="n">
-        <v>0.05470456574121418</v>
+        <v>0.1873340970230239</v>
       </c>
       <c r="T77" t="n">
-        <v>0.05042629453061843</v>
+        <v>0.1735350396016555</v>
       </c>
       <c r="U77" t="n">
-        <v>0.0464826133913158</v>
+        <v>0.1607524228002498</v>
       </c>
       <c r="V77" t="n">
-        <v>0.04055140982840021</v>
+        <v>0.1465270704428882</v>
       </c>
       <c r="W77" t="n">
-        <v>0.035377030659341</v>
+        <v>0.133560552298822</v>
       </c>
       <c r="X77" t="n">
-        <v>0.03086290473174721</v>
+        <v>0.1217414712274566</v>
       </c>
       <c r="Y77" t="n">
-        <v>0.02692478341817532</v>
+        <v>0.1109682878778899</v>
       </c>
       <c r="Z77" t="n">
-        <v>0.02348916825608877</v>
+        <v>0.1011484483503846</v>
       </c>
       <c r="AA77" t="n">
-        <v>0.02020469288131699</v>
+        <v>0.09524428559621646</v>
       </c>
       <c r="AB77" t="n">
-        <v>0.01737948359761618</v>
+        <v>0.08968475628325492</v>
       </c>
       <c r="AC77" t="n">
-        <v>0.01494932152119511</v>
+        <v>0.08444974372201447</v>
       </c>
       <c r="AD77" t="n">
-        <v>0.01285896745371196</v>
+        <v>0.07952030545959678</v>
       </c>
       <c r="AE77" t="n">
-        <v>0.01106090625860086</v>
+        <v>0.07487860473801727</v>
       </c>
       <c r="AF77" t="n">
-        <v>0.008635703729905051</v>
+        <v>0.06978712467373246</v>
       </c>
       <c r="AG77" t="n">
-        <v>0.006320857992482552</v>
+        <v>0.06504184723082007</v>
       </c>
       <c r="AH77" t="n">
-        <v>0.004112461166208455</v>
+        <v>0.06061923185652687</v>
       </c>
       <c r="AI77" t="n">
-        <v>0.002006729568638458</v>
+        <v>0.05649733867235725</v>
       </c>
       <c r="AJ77" t="n">
-        <v>-5.486910640598821e-19</v>
+        <v>0.0526557196338897</v>
       </c>
     </row>
     <row r="78">
@@ -16658,100 +16658,100 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.3513186747284118</v>
+        <v>0.8654174715127384</v>
       </c>
       <c r="F78" t="n">
-        <v>0.320414108207593</v>
+        <v>0.7896239356482596</v>
       </c>
       <c r="G78" t="n">
-        <v>0.2922281339522666</v>
+        <v>0.7204684216263471</v>
       </c>
       <c r="H78" t="n">
-        <v>0.266521604653862</v>
+        <v>0.6573695693945925</v>
       </c>
       <c r="I78" t="n">
-        <v>0.2430764101545143</v>
+        <v>0.5997969345978468</v>
       </c>
       <c r="J78" t="n">
-        <v>0.2216936268650426</v>
+        <v>0.5472665293653507</v>
       </c>
       <c r="K78" t="n">
-        <v>0.202191829973691</v>
+        <v>0.4993367536371391</v>
       </c>
       <c r="L78" t="n">
-        <v>0.1784842648810296</v>
+        <v>0.4429252817014012</v>
       </c>
       <c r="M78" t="n">
-        <v>0.1575564789846687</v>
+        <v>0.3928867717853368</v>
       </c>
       <c r="N78" t="n">
-        <v>0.1390825352957194</v>
+        <v>0.3485012525159161</v>
       </c>
       <c r="O78" t="n">
-        <v>0.1227747138609726</v>
+        <v>0.3091300897030995</v>
       </c>
       <c r="P78" t="n">
-        <v>0.1083790307071547</v>
+        <v>0.274206797450411</v>
       </c>
       <c r="Q78" t="n">
-        <v>0.09652813666745219</v>
+        <v>0.2506547897118108</v>
       </c>
       <c r="R78" t="n">
-        <v>0.08597309929507624</v>
+        <v>0.2291256970638528</v>
       </c>
       <c r="S78" t="n">
-        <v>0.0765722208837923</v>
+        <v>0.2094457684824472</v>
       </c>
       <c r="T78" t="n">
-        <v>0.06819929791006238</v>
+        <v>0.1914561766634926</v>
       </c>
       <c r="U78" t="n">
-        <v>0.06074192679462854</v>
+        <v>0.1750117362035626</v>
       </c>
       <c r="V78" t="n">
-        <v>0.05262902939033064</v>
+        <v>0.1587045456671741</v>
       </c>
       <c r="W78" t="n">
-        <v>0.04559971803221136</v>
+        <v>0.1439168215903422</v>
       </c>
       <c r="X78" t="n">
-        <v>0.03950926529910909</v>
+        <v>0.1305069835876188</v>
       </c>
       <c r="Y78" t="n">
-        <v>0.03423227405425441</v>
+        <v>0.1183466434078195</v>
       </c>
       <c r="Z78" t="n">
-        <v>0.02966009562703773</v>
+        <v>0.1073193757213337</v>
       </c>
       <c r="AA78" t="n">
-        <v>0.02595934639725287</v>
+        <v>0.100348469730741</v>
       </c>
       <c r="AB78" t="n">
-        <v>0.02243897865590657</v>
+        <v>0.09383035737599517</v>
       </c>
       <c r="AC78" t="n">
-        <v>0.01909189002952162</v>
+        <v>0.08773562754798929</v>
       </c>
       <c r="AD78" t="n">
-        <v>0.01591123181772701</v>
+        <v>0.08203677952961501</v>
       </c>
       <c r="AE78" t="n">
-        <v>0.01289040042726198</v>
+        <v>0.07670809890667839</v>
       </c>
       <c r="AF78" t="n">
-        <v>0.01006406495517637</v>
+        <v>0.07114790002780567</v>
       </c>
       <c r="AG78" t="n">
-        <v>0.00736633948991318</v>
+        <v>0.06599073305838268</v>
       </c>
       <c r="AH78" t="n">
-        <v>0.004792669780812099</v>
+        <v>0.06120738416567192</v>
       </c>
       <c r="AI78" t="n">
-        <v>0.002338646317417441</v>
+        <v>0.05677075708629751</v>
       </c>
       <c r="AJ78" t="n">
-        <v>0</v>
+        <v>0.05265571963388967</v>
       </c>
     </row>
     <row r="79">
@@ -16878,100 +16878,100 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.02556092647558943</v>
+        <v>0.345355371448485</v>
       </c>
       <c r="F80" t="n">
-        <v>0.02394915174413385</v>
+        <v>0.3144427907353802</v>
       </c>
       <c r="G80" t="n">
-        <v>0.02243900939237467</v>
+        <v>0.286297179136832</v>
       </c>
       <c r="H80" t="n">
-        <v>0.02102409086928972</v>
+        <v>0.2606708666782123</v>
       </c>
       <c r="I80" t="n">
-        <v>0.01969839172269157</v>
+        <v>0.23733835219625</v>
       </c>
       <c r="J80" t="n">
-        <v>0.01845628611829305</v>
+        <v>0.2160943190201907</v>
       </c>
       <c r="K80" t="n">
-        <v>0.01729250296550367</v>
+        <v>0.1967518282683088</v>
       </c>
       <c r="L80" t="n">
-        <v>0.01506423031208711</v>
+        <v>0.1723440334267647</v>
       </c>
       <c r="M80" t="n">
-        <v>0.0131230878114234</v>
+        <v>0.1509641161621167</v>
       </c>
       <c r="N80" t="n">
-        <v>0.01143207652422497</v>
+        <v>0.1322364570183594</v>
       </c>
       <c r="O80" t="n">
-        <v>0.009958965110480359</v>
+        <v>0.1158320335276901</v>
       </c>
       <c r="P80" t="n">
-        <v>0.008675675487440722</v>
+        <v>0.1014626396811065</v>
       </c>
       <c r="Q80" t="n">
-        <v>0.008138445201162352</v>
+        <v>0.09326452635036973</v>
       </c>
       <c r="R80" t="n">
-        <v>0.007634482224260936</v>
+        <v>0.08572881508599788</v>
       </c>
       <c r="S80" t="n">
-        <v>0.007161726520469998</v>
+        <v>0.07880198424467826</v>
       </c>
       <c r="T80" t="n">
-        <v>0.006718245618676324</v>
+        <v>0.0724348366960313</v>
       </c>
       <c r="U80" t="n">
-        <v>0.006302226713608382</v>
+        <v>0.06658215040486186</v>
       </c>
       <c r="V80" t="n">
-        <v>0.005437392081352883</v>
+        <v>0.05979927240371912</v>
       </c>
       <c r="W80" t="n">
-        <v>0.004603904763098525</v>
+        <v>0.05370738190746518</v>
       </c>
       <c r="X80" t="n">
-        <v>0.003800870770626586</v>
+        <v>0.0482360864172475</v>
       </c>
       <c r="Y80" t="n">
-        <v>0.003027419067225932</v>
+        <v>0.0433221644812435</v>
       </c>
       <c r="Z80" t="n">
-        <v>0.002282701012410389</v>
+        <v>0.03890883516347703</v>
       </c>
       <c r="AA80" t="n">
-        <v>0.002010542729589665</v>
+        <v>0.03697688701273937</v>
       </c>
       <c r="AB80" t="n">
-        <v>0.001748613934053263</v>
+        <v>0.03514086626875796</v>
       </c>
       <c r="AC80" t="n">
-        <v>0.001496608967077074</v>
+        <v>0.03339600982887735</v>
       </c>
       <c r="AD80" t="n">
-        <v>0.001254230415862992</v>
+        <v>0.03173779109372797</v>
       </c>
       <c r="AE80" t="n">
-        <v>0.001021188903644089</v>
+        <v>0.03016190822408139</v>
       </c>
       <c r="AF80" t="n">
-        <v>0.00080171657216371</v>
+        <v>0.02863920714974387</v>
       </c>
       <c r="AG80" t="n">
-        <v>0.0005900745871322383</v>
+        <v>0.02719337848495561</v>
       </c>
       <c r="AH80" t="n">
-        <v>0.000386047228568931</v>
+        <v>0.02582054138438886</v>
       </c>
       <c r="AI80" t="n">
-        <v>0.0001894240990067671</v>
+        <v>0.02451701092425058</v>
       </c>
       <c r="AJ80" t="n">
-        <v>0</v>
+        <v>0.02327928821133234</v>
       </c>
     </row>
     <row r="81">
@@ -16984,100 +16984,100 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.1787370383682185</v>
+        <v>0.4985314833411141</v>
       </c>
       <c r="F81" t="n">
-        <v>0.1603621553471062</v>
+        <v>0.4508383690817707</v>
       </c>
       <c r="G81" t="n">
-        <v>0.1438762838544495</v>
+        <v>0.4077079218229352</v>
       </c>
       <c r="H81" t="n">
-        <v>0.1290852259434892</v>
+        <v>0.3687036439594331</v>
       </c>
       <c r="I81" t="n">
-        <v>0.1158147479937594</v>
+        <v>0.3334307963925294</v>
       </c>
       <c r="J81" t="n">
-        <v>0.1039085282984278</v>
+        <v>0.3015324036102789</v>
       </c>
       <c r="K81" t="n">
-        <v>0.09322631564787377</v>
+        <v>0.2726856409506789</v>
       </c>
       <c r="L81" t="n">
-        <v>0.07817398125748648</v>
+        <v>0.2390193860291384</v>
       </c>
       <c r="M81" t="n">
-        <v>0.06367357040386797</v>
+        <v>0.2065631370620469</v>
       </c>
       <c r="N81" t="n">
-        <v>0.04970927524285668</v>
+        <v>0.1752824915380644</v>
       </c>
       <c r="O81" t="n">
-        <v>0.03626569469369967</v>
+        <v>0.1451439288098047</v>
       </c>
       <c r="P81" t="n">
-        <v>0.02332782458374502</v>
+        <v>0.1161147887774109</v>
       </c>
       <c r="Q81" t="n">
-        <v>0.02228850894213577</v>
+        <v>0.1074669236342285</v>
       </c>
       <c r="R81" t="n">
-        <v>0.02129549753258278</v>
+        <v>0.09946312435313043</v>
       </c>
       <c r="S81" t="n">
-        <v>0.02034672738035492</v>
+        <v>0.09205542292954751</v>
       </c>
       <c r="T81" t="n">
-        <v>0.01944022742164478</v>
+        <v>0.08519942386538507</v>
       </c>
       <c r="U81" t="n">
-        <v>0.01857411440869649</v>
+        <v>0.07885403809994995</v>
       </c>
       <c r="V81" t="n">
-        <v>0.01592571566438206</v>
+        <v>0.06981329404606058</v>
       </c>
       <c r="W81" t="n">
-        <v>0.01337358845510744</v>
+        <v>0.06180908604051329</v>
       </c>
       <c r="X81" t="n">
-        <v>0.01091498433148556</v>
+        <v>0.05472257353510666</v>
       </c>
       <c r="Y81" t="n">
-        <v>0.008547225444224527</v>
+        <v>0.04844854124428156</v>
       </c>
       <c r="Z81" t="n">
-        <v>0.006267702835474046</v>
+        <v>0.04289383698654069</v>
       </c>
       <c r="AA81" t="n">
-        <v>0.005476270299228615</v>
+        <v>0.04053619128486918</v>
       </c>
       <c r="AB81" t="n">
-        <v>0.004784773174069168</v>
+        <v>0.03830813280703019</v>
       </c>
       <c r="AC81" t="n">
-        <v>0.004180592460988783</v>
+        <v>0.03620253883370726</v>
       </c>
       <c r="AD81" t="n">
-        <v>0.003652702581512927</v>
+        <v>0.0342126781435184</v>
       </c>
       <c r="AE81" t="n">
-        <v>0.003191470174023021</v>
+        <v>0.03233218949446033</v>
       </c>
       <c r="AF81" t="n">
-        <v>0.00280701659580277</v>
+        <v>0.03070109684592823</v>
       </c>
       <c r="AG81" t="n">
-        <v>0.00246887538954495</v>
+        <v>0.02915228947623725</v>
       </c>
       <c r="AH81" t="n">
-        <v>0.002171467635145042</v>
+        <v>0.02768161626183223</v>
       </c>
       <c r="AI81" t="n">
-        <v>0.001909886465088664</v>
+        <v>0.02628513549482765</v>
       </c>
       <c r="AJ81" t="n">
-        <v>0.001679816107084288</v>
+        <v>0.02495910431841663</v>
       </c>
     </row>
     <row r="82">
@@ -19172,100 +19172,100 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.1948421286442454</v>
+        <v>0.832433097526288</v>
       </c>
       <c r="F101" t="n">
-        <v>0.1857545624812359</v>
+        <v>0.765428814566991</v>
       </c>
       <c r="G101" t="n">
-        <v>0.177090846433916</v>
+        <v>0.7038178466359298</v>
       </c>
       <c r="H101" t="n">
-        <v>0.168831211851654</v>
+        <v>0.6471660745140174</v>
       </c>
       <c r="I101" t="n">
-        <v>0.1609568121068004</v>
+        <v>0.5950743221470648</v>
       </c>
       <c r="J101" t="n">
-        <v>0.1534496795909247</v>
+        <v>0.5471755439972752</v>
       </c>
       <c r="K101" t="n">
-        <v>0.1462926847167758</v>
+        <v>0.5031322387907053</v>
       </c>
       <c r="L101" t="n">
-        <v>0.1311013592176909</v>
+        <v>0.4434734827839135</v>
       </c>
       <c r="M101" t="n">
-        <v>0.1174875313964013</v>
+        <v>0.3908887460783545</v>
       </c>
       <c r="N101" t="n">
-        <v>0.1052873907333049</v>
+        <v>0.3445392289332405</v>
       </c>
       <c r="O101" t="n">
-        <v>0.09435413712137257</v>
+        <v>0.3036855920382953</v>
       </c>
       <c r="P101" t="n">
-        <v>0.084556214470824</v>
+        <v>0.2676761630227013</v>
       </c>
       <c r="Q101" t="n">
-        <v>0.07279673917572065</v>
+        <v>0.2409643805507453</v>
       </c>
       <c r="R101" t="n">
-        <v>0.06267268784184325</v>
+        <v>0.2169182045891776</v>
       </c>
       <c r="S101" t="n">
-        <v>0.05395661736770702</v>
+        <v>0.1952716304984471</v>
       </c>
       <c r="T101" t="n">
-        <v>0.04645271581636889</v>
+        <v>0.1757851986177856</v>
       </c>
       <c r="U101" t="n">
-        <v>0.03999240337864107</v>
+        <v>0.1582433453042739</v>
       </c>
       <c r="V101" t="n">
-        <v>0.03761655539141614</v>
+        <v>0.144474953442363</v>
       </c>
       <c r="W101" t="n">
-        <v>0.03538185055092732</v>
+        <v>0.131904517893235</v>
       </c>
       <c r="X101" t="n">
-        <v>0.03327990389821354</v>
+        <v>0.120427807215649</v>
       </c>
       <c r="Y101" t="n">
-        <v>0.03130282860361303</v>
+        <v>0.1099496589078798</v>
       </c>
       <c r="Z101" t="n">
-        <v>0.02944320637415582</v>
+        <v>0.1003831903400149</v>
       </c>
       <c r="AA101" t="n">
-        <v>0.02608505445420527</v>
+        <v>0.09330156051589436</v>
       </c>
       <c r="AB101" t="n">
-        <v>0.02280451276762901</v>
+        <v>0.08671951115734793</v>
       </c>
       <c r="AC101" t="n">
-        <v>0.01960018679677348</v>
+        <v>0.08060179887439585</v>
       </c>
       <c r="AD101" t="n">
-        <v>0.01647070450671209</v>
+        <v>0.07491566655629245</v>
       </c>
       <c r="AE101" t="n">
-        <v>0.0134147160041289</v>
+        <v>0.06963066797453858</v>
       </c>
       <c r="AF101" t="n">
-        <v>0.0106082893298346</v>
+        <v>0.06373020362057953</v>
       </c>
       <c r="AG101" t="n">
-        <v>0.007864670024800933</v>
+        <v>0.05832974135772596</v>
       </c>
       <c r="AH101" t="n">
-        <v>0.005182784282144991</v>
+        <v>0.05338691128487984</v>
       </c>
       <c r="AI101" t="n">
-        <v>0.002561574690725413</v>
+        <v>0.04886293390296538</v>
       </c>
       <c r="AJ101" t="n">
-        <v>1.033819963170107e-18</v>
+        <v>0.04472231586624439</v>
       </c>
     </row>
     <row r="102">
@@ -19278,100 +19278,100 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.3152881677079904</v>
+        <v>0.9528791365900331</v>
       </c>
       <c r="F102" t="n">
-        <v>0.2975902658907691</v>
+        <v>0.877151139405974</v>
       </c>
       <c r="G102" t="n">
-        <v>0.2808857909154396</v>
+        <v>0.8074414601148128</v>
       </c>
       <c r="H102" t="n">
-        <v>0.2651189792852675</v>
+        <v>0.7432718059898589</v>
       </c>
       <c r="I102" t="n">
-        <v>0.2502371976460079</v>
+        <v>0.6842018955787473</v>
       </c>
       <c r="J102" t="n">
-        <v>0.2361907670832938</v>
+        <v>0.6298264378400736</v>
       </c>
       <c r="K102" t="n">
-        <v>0.2229327972826454</v>
+        <v>0.5797723513565751</v>
       </c>
       <c r="L102" t="n">
-        <v>0.197692629729294</v>
+        <v>0.5100019928890573</v>
       </c>
       <c r="M102" t="n">
-        <v>0.1753101218199543</v>
+        <v>0.4486278659929414</v>
       </c>
       <c r="N102" t="n">
-        <v>0.155461732967039</v>
+        <v>0.3946395601421953</v>
       </c>
       <c r="O102" t="n">
-        <v>0.1378605534364761</v>
+        <v>0.3471482585784712</v>
       </c>
       <c r="P102" t="n">
-        <v>0.1222521570490986</v>
+        <v>0.3053721056009758</v>
       </c>
       <c r="Q102" t="n">
-        <v>0.107506826870649</v>
+        <v>0.2755093231993295</v>
       </c>
       <c r="R102" t="n">
-        <v>0.09453999097254312</v>
+        <v>0.2485668657272082</v>
       </c>
       <c r="S102" t="n">
-        <v>0.08313713792187731</v>
+        <v>0.2242591503618427</v>
       </c>
       <c r="T102" t="n">
-        <v>0.07310962938264519</v>
+        <v>0.2023285218401118</v>
       </c>
       <c r="U102" t="n">
-        <v>0.06429157945622772</v>
+        <v>0.1825425213818606</v>
       </c>
       <c r="V102" t="n">
-        <v>0.05814645097099899</v>
+        <v>0.1649099558358887</v>
       </c>
       <c r="W102" t="n">
-        <v>0.05258868718297263</v>
+        <v>0.1489805954685207</v>
       </c>
       <c r="X102" t="n">
-        <v>0.04756214650156208</v>
+        <v>0.1345899203820218</v>
       </c>
       <c r="Y102" t="n">
-        <v>0.04301605347106865</v>
+        <v>0.1215893023616389</v>
       </c>
       <c r="Z102" t="n">
-        <v>0.03890448586388055</v>
+        <v>0.1098444698297396</v>
       </c>
       <c r="AA102" t="n">
-        <v>0.03408763901204154</v>
+        <v>0.1009836516299641</v>
       </c>
       <c r="AB102" t="n">
-        <v>0.02938261036543039</v>
+        <v>0.09283760859630462</v>
       </c>
       <c r="AC102" t="n">
-        <v>0.02478738755051674</v>
+        <v>0.08534868199718829</v>
       </c>
       <c r="AD102" t="n">
-        <v>0.02029999066425094</v>
+        <v>0.07846386425497744</v>
       </c>
       <c r="AE102" t="n">
-        <v>0.01591847178116441</v>
+        <v>0.07213442375157413</v>
       </c>
       <c r="AF102" t="n">
-        <v>0.0125882466905318</v>
+        <v>0.06555697570331742</v>
       </c>
       <c r="AG102" t="n">
-        <v>0.009332551491916053</v>
+        <v>0.0595792804579182</v>
       </c>
       <c r="AH102" t="n">
-        <v>0.006150111960461505</v>
+        <v>0.05414665063177473</v>
       </c>
       <c r="AI102" t="n">
-        <v>0.003039673327195816</v>
+        <v>0.04920938541227081</v>
       </c>
       <c r="AJ102" t="n">
-        <v>0</v>
+        <v>0.04472231586624439</v>
       </c>
     </row>
     <row r="103">
@@ -19498,100 +19498,100 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>1.529717891514712</v>
+        <v>4.734675073055096</v>
       </c>
       <c r="F104" t="n">
-        <v>1.412800594834692</v>
+        <v>4.338249373026925</v>
       </c>
       <c r="G104" t="n">
-        <v>1.304819360378165</v>
+        <v>3.975015673129277</v>
       </c>
       <c r="H104" t="n">
-        <v>1.205091199311743</v>
+        <v>3.642194867788052</v>
       </c>
       <c r="I104" t="n">
-        <v>1.112985324066408</v>
+        <v>3.337240540865206</v>
       </c>
       <c r="J104" t="n">
-        <v>1.027919158562173</v>
+        <v>3.057819482997084</v>
       </c>
       <c r="K104" t="n">
-        <v>0.9493546533737776</v>
+        <v>2.801793840180434</v>
       </c>
       <c r="L104" t="n">
-        <v>0.8577092870371286</v>
+        <v>2.506441694232525</v>
       </c>
       <c r="M104" t="n">
-        <v>0.7749108496549341</v>
+        <v>2.242224205255101</v>
       </c>
       <c r="N104" t="n">
-        <v>0.7001053083933063</v>
+        <v>2.005859301734651</v>
       </c>
       <c r="O104" t="n">
-        <v>0.6325210739516012</v>
+        <v>1.794410892954242</v>
       </c>
       <c r="P104" t="n">
-        <v>0.5714610419267491</v>
+        <v>1.605252397298399</v>
       </c>
       <c r="Q104" t="n">
-        <v>0.5267688797548024</v>
+        <v>1.486396224109989</v>
       </c>
       <c r="R104" t="n">
-        <v>0.4855719503512507</v>
+        <v>1.376340405263842</v>
       </c>
       <c r="S104" t="n">
-        <v>0.4475969026068267</v>
+        <v>1.274433344511553</v>
       </c>
       <c r="T104" t="n">
-        <v>0.4125917633386812</v>
+        <v>1.18007169112466</v>
       </c>
       <c r="U104" t="n">
-        <v>0.3803242653903164</v>
+        <v>1.0926967676976</v>
       </c>
       <c r="V104" t="n">
-        <v>0.3317947083502267</v>
+        <v>0.9927301139441241</v>
       </c>
       <c r="W104" t="n">
-        <v>0.2894575458555925</v>
+        <v>0.9019090275228591</v>
       </c>
       <c r="X104" t="n">
-        <v>0.2525226254190354</v>
+        <v>0.8193968154098061</v>
       </c>
       <c r="Y104" t="n">
-        <v>0.2203006183861433</v>
+        <v>0.7444333304300081</v>
       </c>
       <c r="Z104" t="n">
-        <v>0.1921901547664598</v>
+        <v>0.6763279683701852</v>
       </c>
       <c r="AA104" t="n">
-        <v>0.1653163283405119</v>
+        <v>0.6336827784280153</v>
       </c>
       <c r="AB104" t="n">
-        <v>0.142200251876572</v>
+        <v>0.5937265386849422</v>
       </c>
       <c r="AC104" t="n">
-        <v>0.1223164816007183</v>
+        <v>0.5562897000503645</v>
       </c>
       <c r="AD104" t="n">
-        <v>0.1052130462058892</v>
+        <v>0.5212134041835997</v>
       </c>
       <c r="AE104" t="n">
-        <v>0.09050117324383179</v>
+        <v>0.4883488093992412</v>
       </c>
       <c r="AF104" t="n">
-        <v>0.07065798236331874</v>
+        <v>0.451053799973871</v>
       </c>
       <c r="AG104" t="n">
-        <v>0.05171773911224545</v>
+        <v>0.4166069959731224</v>
       </c>
       <c r="AH104" t="n">
-        <v>0.03364846891927651</v>
+        <v>0.384790881051891</v>
       </c>
       <c r="AI104" t="n">
-        <v>0.01641921340791128</v>
+        <v>0.355404550504099</v>
       </c>
       <c r="AJ104" t="n">
-        <v>0</v>
+        <v>0.3282624426382567</v>
       </c>
     </row>
     <row r="105">
@@ -19604,100 +19604,100 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>1.726044137605855</v>
+        <v>4.93100131914624</v>
       </c>
       <c r="F105" t="n">
-        <v>1.589349731326689</v>
+        <v>4.514664607192782</v>
       </c>
       <c r="G105" t="n">
-        <v>1.463480865542641</v>
+        <v>4.133480239864984</v>
       </c>
       <c r="H105" t="n">
-        <v>1.347580209436734</v>
+        <v>3.784480217231053</v>
       </c>
       <c r="I105" t="n">
-        <v>1.240858328675321</v>
+        <v>3.464947134979173</v>
       </c>
       <c r="J105" t="n">
-        <v>1.142588308332675</v>
+        <v>3.172393026005714</v>
       </c>
       <c r="K105" t="n">
-        <v>1.052100801654142</v>
+        <v>2.904539988460799</v>
       </c>
       <c r="L105" t="n">
-        <v>0.9457168444949982</v>
+        <v>2.594311295377884</v>
       </c>
       <c r="M105" t="n">
-        <v>0.8500899804994034</v>
+        <v>2.317217571134884</v>
       </c>
       <c r="N105" t="n">
-        <v>0.7641324981700676</v>
+        <v>2.069719729294913</v>
       </c>
       <c r="O105" t="n">
-        <v>0.6868666707689044</v>
+        <v>1.848656686879255</v>
       </c>
       <c r="P105" t="n">
-        <v>0.6174136351260858</v>
+        <v>1.651204990497736</v>
       </c>
       <c r="Q105" t="n">
-        <v>0.5653153634603569</v>
+        <v>1.525042489338772</v>
       </c>
       <c r="R105" t="n">
-        <v>0.5176132206718302</v>
+        <v>1.408519600941568</v>
       </c>
       <c r="S105" t="n">
-        <v>0.4739362549326028</v>
+        <v>1.300899797943851</v>
       </c>
       <c r="T105" t="n">
-        <v>0.4339448158762326</v>
+        <v>1.201502828330578</v>
       </c>
       <c r="U105" t="n">
-        <v>0.3973279133343284</v>
+        <v>1.109700415641611</v>
       </c>
       <c r="V105" t="n">
-        <v>0.3462015884616911</v>
+        <v>1.007247053919749</v>
       </c>
       <c r="W105" t="n">
-        <v>0.3016539634670638</v>
+        <v>0.9142527238249427</v>
       </c>
       <c r="X105" t="n">
-        <v>0.2628385215669156</v>
+        <v>0.8298441179535309</v>
       </c>
       <c r="Y105" t="n">
-        <v>0.2290176718563982</v>
+        <v>0.7532285572210468</v>
       </c>
       <c r="Z105" t="n">
-        <v>0.1995487332292423</v>
+        <v>0.6836865468329679</v>
       </c>
       <c r="AA105" t="n">
-        <v>0.1711744658460747</v>
+        <v>0.6397625498830706</v>
       </c>
       <c r="AB105" t="n">
-        <v>0.1468347971120832</v>
+        <v>0.598660485757494</v>
       </c>
       <c r="AC105" t="n">
-        <v>0.1259560386905746</v>
+        <v>0.5601990570922016</v>
       </c>
       <c r="AD105" t="n">
-        <v>0.1080460762343096</v>
+        <v>0.5242086141194151</v>
       </c>
       <c r="AE105" t="n">
-        <v>0.09268277020293288</v>
+        <v>0.4905304063583423</v>
       </c>
       <c r="AF105" t="n">
-        <v>0.07236124469611442</v>
+        <v>0.4526650725292701</v>
       </c>
       <c r="AG105" t="n">
-        <v>0.05296443303161459</v>
+        <v>0.4177226635329955</v>
       </c>
       <c r="AH105" t="n">
-        <v>0.03445958986767486</v>
+        <v>0.3854775511044475</v>
       </c>
       <c r="AI105" t="n">
-        <v>0.01681501055349106</v>
+        <v>0.3557215238185052</v>
       </c>
       <c r="AJ105" t="n">
-        <v>-6.841219536810118e-18</v>
+        <v>0.3282624426382568</v>
       </c>
     </row>
     <row r="106">
@@ -19824,100 +19824,100 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0.1136451347052913</v>
+        <v>0.6425359475450803</v>
       </c>
       <c r="F107" t="n">
-        <v>0.1069099613803018</v>
+        <v>0.5875287176178084</v>
       </c>
       <c r="G107" t="n">
-        <v>0.1005739477715226</v>
+        <v>0.5372306333123998</v>
       </c>
       <c r="H107" t="n">
-        <v>0.09461343769798303</v>
+        <v>0.4912385466696276</v>
       </c>
       <c r="I107" t="n">
-        <v>0.08900617696111536</v>
+        <v>0.4491838230560522</v>
       </c>
       <c r="J107" t="n">
-        <v>0.08373123025633669</v>
+        <v>0.4107293864928406</v>
       </c>
       <c r="K107" t="n">
-        <v>0.07876890300886168</v>
+        <v>0.3755670179327316</v>
       </c>
       <c r="L107" t="n">
-        <v>0.06861892108522662</v>
+        <v>0.3287378014924185</v>
       </c>
       <c r="M107" t="n">
-        <v>0.05977684277729289</v>
+        <v>0.2877476907448383</v>
       </c>
       <c r="N107" t="n">
-        <v>0.05207413459595338</v>
+        <v>0.2518686112552123</v>
       </c>
       <c r="O107" t="n">
-        <v>0.04536397989469515</v>
+        <v>0.2204632717344133</v>
       </c>
       <c r="P107" t="n">
-        <v>0.03951848048659118</v>
+        <v>0.192973844345346</v>
       </c>
       <c r="Q107" t="n">
-        <v>0.0370713483162107</v>
+        <v>0.1778739673092611</v>
       </c>
       <c r="R107" t="n">
-        <v>0.03477575172578105</v>
+        <v>0.1639556301200834</v>
       </c>
       <c r="S107" t="n">
-        <v>0.03262230706522032</v>
+        <v>0.1511263792825629</v>
       </c>
       <c r="T107" t="n">
-        <v>0.03060221175516865</v>
+        <v>0.139300995631131</v>
       </c>
       <c r="U107" t="n">
-        <v>0.02870720830491508</v>
+        <v>0.1284009282558344</v>
       </c>
       <c r="V107" t="n">
-        <v>0.02476780893614049</v>
+        <v>0.1140438357636858</v>
       </c>
       <c r="W107" t="n">
-        <v>0.02097119939606044</v>
+        <v>0.101292075161486</v>
       </c>
       <c r="X107" t="n">
-        <v>0.01731330748810328</v>
+        <v>0.08996614698036297</v>
       </c>
       <c r="Y107" t="n">
-        <v>0.01379016556187431</v>
+        <v>0.07990662240445237</v>
       </c>
       <c r="Z107" t="n">
-        <v>0.01039790798379356</v>
+        <v>0.07097189907978839</v>
       </c>
       <c r="AA107" t="n">
-        <v>0.009158202579357356</v>
+        <v>0.06690696922643161</v>
       </c>
       <c r="AB107" t="n">
-        <v>0.007965093407597041</v>
+        <v>0.06307485905138349</v>
       </c>
       <c r="AC107" t="n">
-        <v>0.006817188165591453</v>
+        <v>0.05946223376054839</v>
       </c>
       <c r="AD107" t="n">
-        <v>0.005713132111352434</v>
+        <v>0.0560565223128556</v>
       </c>
       <c r="AE107" t="n">
-        <v>0.004651607107735087</v>
+        <v>0.0528458736761506</v>
       </c>
       <c r="AF107" t="n">
-        <v>0.003651890940214792</v>
+        <v>0.04960230138251124</v>
       </c>
       <c r="AG107" t="n">
-        <v>0.002687842703542342</v>
+        <v>0.0465578129622607</v>
       </c>
       <c r="AH107" t="n">
-        <v>0.0017584797738446</v>
+        <v>0.04370018905197639</v>
       </c>
       <c r="AI107" t="n">
-        <v>0.0008628437717761267</v>
+        <v>0.0410179602879213</v>
       </c>
       <c r="AJ107" t="n">
-        <v>2.610323415271306e-19</v>
+        <v>0.03850036127258807</v>
       </c>
     </row>
     <row r="108">
@@ -19930,100 +19930,100 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.2188768580838302</v>
+        <v>0.7477676709236192</v>
       </c>
       <c r="F108" t="n">
-        <v>0.2001735939093283</v>
+        <v>0.6805305560909338</v>
       </c>
       <c r="G108" t="n">
-        <v>0.1830685438806417</v>
+        <v>0.6193392089302309</v>
       </c>
       <c r="H108" t="n">
-        <v>0.16742513887101</v>
+        <v>0.563650011428832</v>
       </c>
       <c r="I108" t="n">
-        <v>0.1531184797332137</v>
+        <v>0.5129682261397273</v>
       </c>
       <c r="J108" t="n">
-        <v>0.1400343400872053</v>
+        <v>0.4668436009819236</v>
       </c>
       <c r="K108" t="n">
-        <v>0.1280682543206144</v>
+        <v>0.4248663692444844</v>
       </c>
       <c r="L108" t="n">
-        <v>0.1110659298363989</v>
+        <v>0.3663373092578176</v>
       </c>
       <c r="M108" t="n">
-        <v>0.09467836170606189</v>
+        <v>0.3158711394194449</v>
       </c>
       <c r="N108" t="n">
-        <v>0.07888803246762149</v>
+        <v>0.2723571260603434</v>
       </c>
       <c r="O108" t="n">
-        <v>0.06367787421755537</v>
+        <v>0.2348375487934286</v>
       </c>
       <c r="P108" t="n">
-        <v>0.04903125773633135</v>
+        <v>0.2024866215950862</v>
       </c>
       <c r="Q108" t="n">
-        <v>0.04626489239608279</v>
+        <v>0.1870939652974845</v>
       </c>
       <c r="R108" t="n">
-        <v>0.04365460661709862</v>
+        <v>0.1728714300974135</v>
       </c>
       <c r="S108" t="n">
-        <v>0.04119159432120471</v>
+        <v>0.1597300655657583</v>
       </c>
       <c r="T108" t="n">
-        <v>0.03886754627306899</v>
+        <v>0.1475876831195554</v>
       </c>
       <c r="U108" t="n">
-        <v>0.03667462204810762</v>
+        <v>0.1363683419990268</v>
       </c>
       <c r="V108" t="n">
-        <v>0.03157725957118211</v>
+        <v>0.1205308336379959</v>
       </c>
       <c r="W108" t="n">
-        <v>0.02666483839498397</v>
+        <v>0.1065326573932674</v>
       </c>
       <c r="X108" t="n">
-        <v>0.02193208233055129</v>
+        <v>0.09416019742597709</v>
       </c>
       <c r="Y108" t="n">
-        <v>0.01737385067052007</v>
+        <v>0.08322464675380657</v>
       </c>
       <c r="Z108" t="n">
-        <v>0.01298513491094617</v>
+        <v>0.07355912600694096</v>
       </c>
       <c r="AA108" t="n">
-        <v>0.01114964171356823</v>
+        <v>0.06921449539237157</v>
       </c>
       <c r="AB108" t="n">
-        <v>0.009573601752581429</v>
+        <v>0.06512647216565057</v>
       </c>
       <c r="AC108" t="n">
-        <v>0.008220340426320139</v>
+        <v>0.0612799002968781</v>
       </c>
       <c r="AD108" t="n">
-        <v>0.007058367213402467</v>
+        <v>0.05766051891838734</v>
       </c>
       <c r="AE108" t="n">
-        <v>0.006060642885265183</v>
+        <v>0.05425490945368072</v>
       </c>
       <c r="AF108" t="n">
-        <v>0.004993277965240873</v>
+        <v>0.05094135071131729</v>
       </c>
       <c r="AG108" t="n">
-        <v>0.00396361401938009</v>
+        <v>0.04783016391371706</v>
       </c>
       <c r="AH108" t="n">
-        <v>0.002970616124050803</v>
+        <v>0.04490898941760477</v>
       </c>
       <c r="AI108" t="n">
-        <v>0.002013274843735563</v>
+        <v>0.04216622243128339</v>
       </c>
       <c r="AJ108" t="n">
-        <v>0.001090605640318604</v>
+        <v>0.03959096691290668</v>
       </c>
     </row>
     <row r="109">
@@ -23100,100 +23100,100 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.1513055075564004</v>
+        <v>0.6859782491779558</v>
       </c>
       <c r="F137" t="n">
-        <v>0.1448968448228416</v>
+        <v>0.6310988648149798</v>
       </c>
       <c r="G137" t="n">
-        <v>0.1387596259956931</v>
+        <v>0.5806099211571841</v>
       </c>
       <c r="H137" t="n">
-        <v>0.1328823538566754</v>
+        <v>0.5341601757515155</v>
       </c>
       <c r="I137" t="n">
-        <v>0.1272540181611528</v>
+        <v>0.4914264861169081</v>
       </c>
       <c r="J137" t="n">
-        <v>0.1218640750119849</v>
+        <v>0.4521115617004633</v>
       </c>
       <c r="K137" t="n">
-        <v>0.1167024271070148</v>
+        <v>0.4159418956808218</v>
       </c>
       <c r="L137" t="n">
-        <v>0.1048459564832042</v>
+        <v>0.3668119962631358</v>
       </c>
       <c r="M137" t="n">
-        <v>0.09419405288630188</v>
+        <v>0.3234851838675953</v>
       </c>
       <c r="N137" t="n">
-        <v>0.08462433742562853</v>
+        <v>0.2852760140014222</v>
       </c>
       <c r="O137" t="n">
-        <v>0.07602686438570325</v>
+        <v>0.2515800049681718</v>
       </c>
       <c r="P137" t="n">
-        <v>0.06830285806848294</v>
+        <v>0.2218640747674981</v>
       </c>
       <c r="Q137" t="n">
-        <v>0.05895207296575744</v>
+        <v>0.1999419097414721</v>
       </c>
       <c r="R137" t="n">
-        <v>0.05088142729657783</v>
+        <v>0.1801858516885193</v>
       </c>
       <c r="S137" t="n">
-        <v>0.0439156676515976</v>
+        <v>0.1623818697675607</v>
       </c>
       <c r="T137" t="n">
-        <v>0.0379035331309444</v>
+        <v>0.146337081308638</v>
       </c>
       <c r="U137" t="n">
-        <v>0.03271447072617453</v>
+        <v>0.1318776621834966</v>
       </c>
       <c r="V137" t="n">
-        <v>0.03084909362420568</v>
+        <v>0.1204675416219593</v>
       </c>
       <c r="W137" t="n">
-        <v>0.02909008020947711</v>
+        <v>0.110044630335088</v>
       </c>
       <c r="X137" t="n">
-        <v>0.02743136563110615</v>
+        <v>0.1005235144881445</v>
       </c>
       <c r="Y137" t="n">
-        <v>0.02586723085563323</v>
+        <v>0.09182617029361939</v>
       </c>
       <c r="Z137" t="n">
-        <v>0.02439228294853369</v>
+        <v>0.08388132462069109</v>
       </c>
       <c r="AA137" t="n">
-        <v>0.02164020830459561</v>
+        <v>0.07802104063447045</v>
       </c>
       <c r="AB137" t="n">
-        <v>0.01895169764719122</v>
+        <v>0.07257017946738688</v>
       </c>
       <c r="AC137" t="n">
-        <v>0.01632560909751594</v>
+        <v>0.06750013720788517</v>
       </c>
       <c r="AD137" t="n">
-        <v>0.01376081918429463</v>
+        <v>0.06278430832778795</v>
       </c>
       <c r="AE137" t="n">
-        <v>0.01125622256451506</v>
+        <v>0.05839794606726022</v>
       </c>
       <c r="AF137" t="n">
-        <v>0.008901363673195595</v>
+        <v>0.05344807798642889</v>
       </c>
       <c r="AG137" t="n">
-        <v>0.006599206138123388</v>
+        <v>0.04891776565485993</v>
       </c>
       <c r="AH137" t="n">
-        <v>0.00434884893319683</v>
+        <v>0.04477144710931218</v>
       </c>
       <c r="AI137" t="n">
-        <v>0.002149404789900836</v>
+        <v>0.04097657465397329</v>
       </c>
       <c r="AJ137" t="n">
-        <v>0</v>
+        <v>0.03750335936814978</v>
       </c>
     </row>
     <row r="138">
@@ -23206,100 +23206,100 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0.2701022948067976</v>
+        <v>0.804775036428353</v>
       </c>
       <c r="F138" t="n">
-        <v>0.2542547767174249</v>
+        <v>0.7401855927748755</v>
       </c>
       <c r="G138" t="n">
-        <v>0.2393370686830634</v>
+        <v>0.6807799533432343</v>
       </c>
       <c r="H138" t="n">
-        <v>0.2252946166256852</v>
+        <v>0.6261420776059015</v>
       </c>
       <c r="I138" t="n">
-        <v>0.2120760672795284</v>
+        <v>0.5758893155171533</v>
       </c>
       <c r="J138" t="n">
-        <v>0.1996330803921368</v>
+        <v>0.5296697276677154</v>
       </c>
       <c r="K138" t="n">
-        <v>0.1879201519439925</v>
+        <v>0.4871596205177996</v>
       </c>
       <c r="L138" t="n">
-        <v>0.1664436226980019</v>
+        <v>0.4283346980270641</v>
       </c>
       <c r="M138" t="n">
-        <v>0.1474215471318453</v>
+        <v>0.3766129330237309</v>
       </c>
       <c r="N138" t="n">
-        <v>0.130573417031302</v>
+        <v>0.3311366134334868</v>
       </c>
       <c r="O138" t="n">
-        <v>0.1156507821748899</v>
+        <v>0.2911515966162775</v>
       </c>
       <c r="P138" t="n">
-        <v>0.1024335865734253</v>
+        <v>0.2559948032724404</v>
       </c>
       <c r="Q138" t="n">
-        <v>0.09017284148426066</v>
+        <v>0.2310476666638653</v>
       </c>
       <c r="R138" t="n">
-        <v>0.07937964112500473</v>
+        <v>0.2085316716918044</v>
       </c>
       <c r="S138" t="n">
-        <v>0.06987832834606174</v>
+        <v>0.1882098993963976</v>
       </c>
       <c r="T138" t="n">
-        <v>0.06151427120652309</v>
+        <v>0.1698685189804398</v>
       </c>
       <c r="U138" t="n">
-        <v>0.05415134637065108</v>
+        <v>0.1533145378279731</v>
       </c>
       <c r="V138" t="n">
-        <v>0.04890249588880445</v>
+        <v>0.1384323359796837</v>
       </c>
       <c r="W138" t="n">
-        <v>0.0441624126533381</v>
+        <v>0.1249947455491435</v>
       </c>
       <c r="X138" t="n">
-        <v>0.0398817822263795</v>
+        <v>0.112861538486124</v>
       </c>
       <c r="Y138" t="n">
-        <v>0.03601607018252736</v>
+        <v>0.1019060986403371</v>
       </c>
       <c r="Z138" t="n">
-        <v>0.03252505878573154</v>
+        <v>0.09201410045788892</v>
       </c>
       <c r="AA138" t="n">
-        <v>0.0285075188292197</v>
+        <v>0.08461109911507302</v>
       </c>
       <c r="AB138" t="n">
-        <v>0.02458323059578103</v>
+        <v>0.07780370679966717</v>
       </c>
       <c r="AC138" t="n">
-        <v>0.02075051592286025</v>
+        <v>0.07154400374276891</v>
       </c>
       <c r="AD138" t="n">
-        <v>0.01700772372514478</v>
+        <v>0.0657879255640713</v>
       </c>
       <c r="AE138" t="n">
-        <v>0.0133532295835396</v>
+        <v>0.06049495308628475</v>
       </c>
       <c r="AF138" t="n">
-        <v>0.01055966618050617</v>
+        <v>0.05497805225157783</v>
       </c>
       <c r="AG138" t="n">
-        <v>0.007828622268829641</v>
+        <v>0.0499642709874668</v>
       </c>
       <c r="AH138" t="n">
-        <v>0.005159028963426536</v>
+        <v>0.04540772677586756</v>
       </c>
       <c r="AI138" t="n">
-        <v>0.002549833699804963</v>
+        <v>0.04126672140316114</v>
       </c>
       <c r="AJ138" t="n">
-        <v>0</v>
+        <v>0.03750335936814977</v>
       </c>
     </row>
     <row r="139">
@@ -23426,100 +23426,100 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>0.2048277868855065</v>
+        <v>0.7694200341753891</v>
       </c>
       <c r="F140" t="n">
-        <v>0.1893473651429064</v>
+        <v>0.7046984790723777</v>
       </c>
       <c r="G140" t="n">
-        <v>0.175036918729204</v>
+        <v>0.6454211280567235</v>
       </c>
       <c r="H140" t="n">
-        <v>0.1618080235502119</v>
+        <v>0.5911300292436544</v>
       </c>
       <c r="I140" t="n">
-        <v>0.1495789384051676</v>
+        <v>0.5414057524359405</v>
       </c>
       <c r="J140" t="n">
-        <v>0.1382740999087348</v>
+        <v>0.4958641487825808</v>
       </c>
       <c r="K140" t="n">
-        <v>0.1278236555856599</v>
+        <v>0.4541533830063364</v>
       </c>
       <c r="L140" t="n">
-        <v>0.1155760481204978</v>
+        <v>0.4060168386780534</v>
       </c>
       <c r="M140" t="n">
-        <v>0.1045019627857537</v>
+        <v>0.3629823743662842</v>
       </c>
       <c r="N140" t="n">
-        <v>0.09448895687010631</v>
+        <v>0.3245092113163807</v>
       </c>
       <c r="O140" t="n">
-        <v>0.08543536152239568</v>
+        <v>0.290113888898956</v>
       </c>
       <c r="P140" t="n">
-        <v>0.07724924943871105</v>
+        <v>0.2593641893573799</v>
       </c>
       <c r="Q140" t="n">
-        <v>0.07126360540742395</v>
+        <v>0.2403116761685118</v>
       </c>
       <c r="R140" t="n">
-        <v>0.06574175791435058</v>
+        <v>0.2226587326724042</v>
       </c>
       <c r="S140" t="n">
-        <v>0.06064776976915107</v>
+        <v>0.2063025485308368</v>
       </c>
       <c r="T140" t="n">
-        <v>0.0559484883681375</v>
+        <v>0.1911478657023416</v>
       </c>
       <c r="U140" t="n">
-        <v>0.05161332993108401</v>
+        <v>0.1771064236615527</v>
       </c>
       <c r="V140" t="n">
-        <v>0.04506221060337754</v>
+        <v>0.1614427938859121</v>
       </c>
       <c r="W140" t="n">
-        <v>0.03934260446234501</v>
+        <v>0.1471644853915436</v>
       </c>
       <c r="X140" t="n">
-        <v>0.03434897012718933</v>
+        <v>0.1341489777231099</v>
       </c>
       <c r="Y140" t="n">
-        <v>0.02998916225609281</v>
+        <v>0.1222845863679385</v>
       </c>
       <c r="Z140" t="n">
-        <v>0.02618273122868305</v>
+        <v>0.1114695044045928</v>
       </c>
       <c r="AA140" t="n">
-        <v>0.02253875877407334</v>
+        <v>0.1049483505866403</v>
       </c>
       <c r="AB140" t="n">
-        <v>0.01940193491041765</v>
+        <v>0.09880869525425616</v>
       </c>
       <c r="AC140" t="n">
-        <v>0.01670167741007556</v>
+        <v>0.09302822010326371</v>
       </c>
       <c r="AD140" t="n">
-        <v>0.01437722730223424</v>
+        <v>0.08758591248788401</v>
       </c>
       <c r="AE140" t="n">
-        <v>0.01237628172457766</v>
+        <v>0.08246198903751942</v>
       </c>
       <c r="AF140" t="n">
-        <v>0.009662671371813116</v>
+        <v>0.07681213206516831</v>
       </c>
       <c r="AG140" t="n">
-        <v>0.007072541564592189</v>
+        <v>0.07154937324774406</v>
       </c>
       <c r="AH140" t="n">
-        <v>0.004601519693271429</v>
+        <v>0.06664719067818232</v>
       </c>
       <c r="AI140" t="n">
-        <v>0.002245372115616442</v>
+        <v>0.06208087958945249</v>
       </c>
       <c r="AJ140" t="n">
-        <v>-6.025820773422404e-19</v>
+        <v>0.05782742785378588</v>
       </c>
     </row>
     <row r="141">
@@ -23532,100 +23532,100 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>0.3860604230775059</v>
+        <v>0.9506526703673883</v>
       </c>
       <c r="F141" t="n">
-        <v>0.3519665227678771</v>
+        <v>0.8672612796205235</v>
       </c>
       <c r="G141" t="n">
-        <v>0.3208835346596515</v>
+        <v>0.79118499381941</v>
       </c>
       <c r="H141" t="n">
-        <v>0.2925455580432525</v>
+        <v>0.7217821308924562</v>
       </c>
       <c r="I141" t="n">
-        <v>0.2667101745236397</v>
+        <v>0.6584672972128786</v>
       </c>
       <c r="J141" t="n">
-        <v>0.2431563742421043</v>
+        <v>0.6007064499681214</v>
       </c>
       <c r="K141" t="n">
-        <v>0.2216826652382763</v>
+        <v>0.5480123926589524</v>
       </c>
       <c r="L141" t="n">
-        <v>0.195677664933751</v>
+        <v>0.4860916099626282</v>
       </c>
       <c r="M141" t="n">
-        <v>0.1727232416335732</v>
+        <v>0.4311673539527205</v>
       </c>
       <c r="N141" t="n">
-        <v>0.1524615403117681</v>
+        <v>0.3824490760679524</v>
       </c>
       <c r="O141" t="n">
-        <v>0.1345766849579479</v>
+        <v>0.3392355530731329</v>
       </c>
       <c r="P141" t="n">
-        <v>0.1187898541313165</v>
+        <v>0.3009047940499853</v>
       </c>
       <c r="Q141" t="n">
-        <v>0.1058791336350633</v>
+        <v>0.2751357371477288</v>
       </c>
       <c r="R141" t="n">
-        <v>0.09437161970852372</v>
+        <v>0.2515735054830969</v>
       </c>
       <c r="S141" t="n">
-        <v>0.08411480431174281</v>
+        <v>0.2300291096938522</v>
       </c>
       <c r="T141" t="n">
-        <v>0.07497275479911832</v>
+        <v>0.2103297451968824</v>
       </c>
       <c r="U141" t="n">
-        <v>0.06682431241635799</v>
+        <v>0.1923174061468266</v>
       </c>
       <c r="V141" t="n">
-        <v>0.05792272864828513</v>
+        <v>0.1744131733749245</v>
       </c>
       <c r="W141" t="n">
-        <v>0.05020691381242835</v>
+        <v>0.1581757764738521</v>
       </c>
       <c r="X141" t="n">
-        <v>0.0435189131001555</v>
+        <v>0.1434500375113471</v>
       </c>
       <c r="Y141" t="n">
-        <v>0.03772181266696514</v>
+        <v>0.1300952252028845</v>
       </c>
       <c r="Z141" t="n">
-        <v>0.0326969367917538</v>
+        <v>0.1179837099676636</v>
       </c>
       <c r="AA141" t="n">
-        <v>0.02770744491381382</v>
+        <v>0.1103312347385891</v>
       </c>
       <c r="AB141" t="n">
-        <v>0.02347934023732898</v>
+        <v>0.1031751024126803</v>
       </c>
       <c r="AC141" t="n">
-        <v>0.01989643648828152</v>
+        <v>0.09648311997131918</v>
       </c>
       <c r="AD141" t="n">
-        <v>0.01686027720245918</v>
+        <v>0.09022518244920961</v>
       </c>
       <c r="AE141" t="n">
-        <v>0.01428743018938048</v>
+        <v>0.0843731375023222</v>
       </c>
       <c r="AF141" t="n">
-        <v>0.01115478345919895</v>
+        <v>0.07823302700556495</v>
       </c>
       <c r="AG141" t="n">
-        <v>0.008164685170743473</v>
+        <v>0.07253975252828548</v>
       </c>
       <c r="AH141" t="n">
-        <v>0.005312087494915079</v>
+        <v>0.06726079634488125</v>
       </c>
       <c r="AI141" t="n">
-        <v>0.002592103029405322</v>
+        <v>0.06236600715150687</v>
       </c>
       <c r="AJ141" t="n">
-        <v>-6.025820773422404e-19</v>
+        <v>0.05782742785378588</v>
       </c>
     </row>
     <row r="142">
@@ -23752,100 +23752,100 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>0.4177347064778237</v>
+        <v>2.016706931342302</v>
       </c>
       <c r="F143" t="n">
-        <v>0.3913939459034382</v>
+        <v>1.844350134298218</v>
       </c>
       <c r="G143" t="n">
-        <v>0.3667141334305099</v>
+        <v>1.686723720249111</v>
       </c>
       <c r="H143" t="n">
-        <v>0.3435905359937978</v>
+        <v>1.542568764760899</v>
       </c>
       <c r="I143" t="n">
-        <v>0.3219250245965113</v>
+        <v>1.410733936714031</v>
       </c>
       <c r="J143" t="n">
-        <v>0.3016256578828911</v>
+        <v>1.290166302897459</v>
       </c>
       <c r="K143" t="n">
-        <v>0.2826062919691171</v>
+        <v>1.179902918483142</v>
       </c>
       <c r="L143" t="n">
-        <v>0.2461902871065209</v>
+        <v>1.032597896312725</v>
       </c>
       <c r="M143" t="n">
-        <v>0.2144667659140957</v>
+        <v>0.9036831749176658</v>
       </c>
       <c r="N143" t="n">
-        <v>0.1868310656047535</v>
+        <v>0.7908628165381714</v>
       </c>
       <c r="O143" t="n">
-        <v>0.1627564388647012</v>
+        <v>0.6921275198464051</v>
       </c>
       <c r="P143" t="n">
-        <v>0.1417840138425313</v>
+        <v>0.60571883481086</v>
       </c>
       <c r="Q143" t="n">
-        <v>0.1330042172195954</v>
+        <v>0.5586991752403329</v>
       </c>
       <c r="R143" t="n">
-        <v>0.1247680984532177</v>
+        <v>0.5153294738006582</v>
       </c>
       <c r="S143" t="n">
-        <v>0.1170419909763459</v>
+        <v>0.4753263980628336</v>
       </c>
       <c r="T143" t="n">
-        <v>0.1097943129817231</v>
+        <v>0.4384286096214718</v>
       </c>
       <c r="U143" t="n">
-        <v>0.1029954383257615</v>
+        <v>0.4043950567820291</v>
       </c>
       <c r="V143" t="n">
-        <v>0.08886170019220366</v>
+        <v>0.3581799296185685</v>
       </c>
       <c r="W143" t="n">
-        <v>0.0752402619952557</v>
+        <v>0.3172463654784811</v>
       </c>
       <c r="X143" t="n">
-        <v>0.06211651354829159</v>
+        <v>0.2809907761065359</v>
       </c>
       <c r="Y143" t="n">
-        <v>0.04947621975442614</v>
+        <v>0.248878552597032</v>
       </c>
       <c r="Z143" t="n">
-        <v>0.03730551153169406</v>
+        <v>0.2204361822870274</v>
       </c>
       <c r="AA143" t="n">
-        <v>0.03285770873009385</v>
+        <v>0.2073669521944126</v>
       </c>
       <c r="AB143" t="n">
-        <v>0.02857708343171189</v>
+        <v>0.1950725711916414</v>
       </c>
       <c r="AC143" t="n">
-        <v>0.02445864034588377</v>
+        <v>0.1835070999917186</v>
       </c>
       <c r="AD143" t="n">
-        <v>0.02049751894268939</v>
+        <v>0.1726273229581214</v>
       </c>
       <c r="AE143" t="n">
-        <v>0.01668899002270364</v>
+        <v>0.1623925866248902</v>
       </c>
       <c r="AF143" t="n">
-        <v>0.01310221823418828</v>
+        <v>0.151929077141497</v>
       </c>
       <c r="AG143" t="n">
-        <v>0.009643415495565449</v>
+        <v>0.1421397673428589</v>
       </c>
       <c r="AH143" t="n">
-        <v>0.006309056358611537</v>
+        <v>0.1329812162385849</v>
       </c>
       <c r="AI143" t="n">
-        <v>0.003095702359379885</v>
+        <v>0.1244127818897947</v>
       </c>
       <c r="AJ143" t="n">
-        <v>7.891675441517908e-19</v>
+        <v>0.1163964410566617</v>
       </c>
     </row>
     <row r="144">
@@ -23858,100 +23858,100 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>0.5819999485367675</v>
+        <v>2.180972173401246</v>
       </c>
       <c r="F144" t="n">
-        <v>0.5382203370107359</v>
+        <v>1.990734992166053</v>
       </c>
       <c r="G144" t="n">
-        <v>0.4977339463693263</v>
+        <v>1.817091413346187</v>
       </c>
       <c r="H144" t="n">
-        <v>0.4602930516232829</v>
+        <v>1.658594045641324</v>
       </c>
       <c r="I144" t="n">
-        <v>0.4256685623276005</v>
+        <v>1.513921747707227</v>
       </c>
       <c r="J144" t="n">
-        <v>0.3936486208406651</v>
+        <v>1.3818686158943</v>
       </c>
       <c r="K144" t="n">
-        <v>0.3640373060261352</v>
+        <v>1.26133393254016</v>
       </c>
       <c r="L144" t="n">
-        <v>0.3196298988245874</v>
+        <v>1.094820062121605</v>
       </c>
       <c r="M144" t="n">
-        <v>0.2768168906736242</v>
+        <v>0.9502883713039181</v>
       </c>
       <c r="N144" t="n">
-        <v>0.235552967669844</v>
+        <v>0.8248369023175143</v>
       </c>
       <c r="O144" t="n">
-        <v>0.1957939772381936</v>
+        <v>0.7159467967509868</v>
       </c>
       <c r="P144" t="n">
-        <v>0.1574969000638193</v>
+        <v>0.6214317210321484</v>
       </c>
       <c r="Q144" t="n">
-        <v>0.1481923370446435</v>
+        <v>0.5739281780684187</v>
       </c>
       <c r="R144" t="n">
-        <v>0.1394374667047696</v>
+        <v>0.5300559054723473</v>
       </c>
       <c r="S144" t="n">
-        <v>0.1311998144356581</v>
+        <v>0.4895373213277157</v>
       </c>
       <c r="T144" t="n">
-        <v>0.1234488241556838</v>
+        <v>0.4521160626616534</v>
       </c>
       <c r="U144" t="n">
-        <v>0.1161557449678759</v>
+        <v>0.4175553634241436</v>
       </c>
       <c r="V144" t="n">
-        <v>0.1001093222324241</v>
+        <v>0.3688889177561463</v>
       </c>
       <c r="W144" t="n">
-        <v>0.08464482382052249</v>
+        <v>0.3258945892285781</v>
       </c>
       <c r="X144" t="n">
-        <v>0.06974565083131951</v>
+        <v>0.2879112875889426</v>
       </c>
       <c r="Y144" t="n">
-        <v>0.05539563055179477</v>
+        <v>0.2543549732364008</v>
       </c>
       <c r="Z144" t="n">
-        <v>0.0415790061450691</v>
+        <v>0.2247096769004025</v>
       </c>
       <c r="AA144" t="n">
-        <v>0.03555698180896629</v>
+        <v>0.2111770305801054</v>
       </c>
       <c r="AB144" t="n">
-        <v>0.03040714708167921</v>
+        <v>0.1984593581361287</v>
       </c>
       <c r="AC144" t="n">
-        <v>0.02600317987095633</v>
+        <v>0.1865075795582983</v>
       </c>
       <c r="AD144" t="n">
-        <v>0.02223705372901322</v>
+        <v>0.1752755705721618</v>
       </c>
       <c r="AE144" t="n">
-        <v>0.01901638803411604</v>
+        <v>0.1647199846363026</v>
       </c>
       <c r="AF144" t="n">
-        <v>0.01531787630644288</v>
+        <v>0.1541412804132552</v>
       </c>
       <c r="AG144" t="n">
-        <v>0.01175069174138408</v>
+        <v>0.1442419654172394</v>
       </c>
       <c r="AH144" t="n">
-        <v>0.008311222503729412</v>
+        <v>0.1349784076766948</v>
       </c>
       <c r="AI144" t="n">
-        <v>0.004995945796660693</v>
+        <v>0.1263097773677349</v>
       </c>
       <c r="AJ144" t="n">
-        <v>0.001801425796981546</v>
+        <v>0.1181978668536433</v>
       </c>
     </row>
     <row r="145">
@@ -24082,100 +24082,100 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>0.1450015920281081</v>
+        <v>0.6598115858562925</v>
       </c>
       <c r="F146" t="n">
-        <v>0.1387317837029338</v>
+        <v>0.6068406986364658</v>
       </c>
       <c r="G146" t="n">
-        <v>0.1327330792731346</v>
+        <v>0.5581224116331299</v>
       </c>
       <c r="H146" t="n">
-        <v>0.1269937563194156</v>
+        <v>0.5133153182822178</v>
       </c>
       <c r="I146" t="n">
-        <v>0.1215025992949997</v>
+        <v>0.4721054207663245</v>
       </c>
       <c r="J146" t="n">
-        <v>0.116248877608672</v>
+        <v>0.434203929590132</v>
       </c>
       <c r="K146" t="n">
-        <v>0.1112223246555035</v>
+        <v>0.3993452398099651</v>
       </c>
       <c r="L146" t="n">
-        <v>0.09981370974215233</v>
+        <v>0.3520389143165714</v>
       </c>
       <c r="M146" t="n">
-        <v>0.08957533196099815</v>
+        <v>0.3103364829193033</v>
       </c>
       <c r="N146" t="n">
-        <v>0.08038715439643171</v>
+        <v>0.273574109889787</v>
       </c>
       <c r="O146" t="n">
-        <v>0.07214145290323234</v>
+        <v>0.2411665972944941</v>
       </c>
       <c r="P146" t="n">
-        <v>0.06474155312581019</v>
+        <v>0.2125980695835427</v>
       </c>
       <c r="Q146" t="n">
-        <v>0.05581837777986304</v>
+        <v>0.1915769877918016</v>
       </c>
       <c r="R146" t="n">
-        <v>0.04812506261505472</v>
+        <v>0.1726344097257089</v>
       </c>
       <c r="S146" t="n">
-        <v>0.04149209890758349</v>
+        <v>0.1555648189527455</v>
       </c>
       <c r="T146" t="n">
-        <v>0.03577334092066476</v>
+        <v>0.1401830199104074</v>
       </c>
       <c r="U146" t="n">
-        <v>0.03084278583921461</v>
+        <v>0.1263221286373943</v>
       </c>
       <c r="V146" t="n">
-        <v>0.02905342289006616</v>
+        <v>0.1153371684712506</v>
       </c>
       <c r="W146" t="n">
-        <v>0.02736787091896866</v>
+        <v>0.1053074593854473</v>
       </c>
       <c r="X146" t="n">
-        <v>0.0257801072689933</v>
+        <v>0.09614993283784218</v>
       </c>
       <c r="Y146" t="n">
-        <v>0.02428445869131008</v>
+        <v>0.0877887439187344</v>
       </c>
       <c r="Z146" t="n">
-        <v>0.02287558107406489</v>
+        <v>0.08015464318448179</v>
       </c>
       <c r="AA146" t="n">
-        <v>0.02028312811685646</v>
+        <v>0.07457837001824927</v>
       </c>
       <c r="AB146" t="n">
-        <v>0.01775056759823787</v>
+        <v>0.06939003223777945</v>
       </c>
       <c r="AC146" t="n">
-        <v>0.01527682349791768</v>
+        <v>0.06456264159141387</v>
       </c>
       <c r="AD146" t="n">
-        <v>0.01286083714228274</v>
+        <v>0.06007108737142091</v>
       </c>
       <c r="AE146" t="n">
-        <v>0.01050156694121867</v>
+        <v>0.05589200579526443</v>
       </c>
       <c r="AF146" t="n">
-        <v>0.008304585836538397</v>
+        <v>0.05121599043625894</v>
       </c>
       <c r="AG146" t="n">
-        <v>0.006156772809101755</v>
+        <v>0.04693117806463144</v>
       </c>
       <c r="AH146" t="n">
-        <v>0.004057287240675798</v>
+        <v>0.04300484000744488</v>
       </c>
       <c r="AI146" t="n">
-        <v>0.002005301348258492</v>
+        <v>0.03940698572533172</v>
       </c>
       <c r="AJ146" t="n">
-        <v>8.347371196180169e-19</v>
+        <v>0.03611013373582281</v>
       </c>
     </row>
     <row r="147">
@@ -24188,100 +24188,100 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>0.2603906999384525</v>
+        <v>0.7752006937666369</v>
       </c>
       <c r="F147" t="n">
-        <v>0.2451043894175941</v>
+        <v>0.7129825542129734</v>
       </c>
       <c r="G147" t="n">
-        <v>0.2307154661282895</v>
+        <v>0.6557580852282948</v>
       </c>
       <c r="H147" t="n">
-        <v>0.2171712486964256</v>
+        <v>0.6031264913865335</v>
       </c>
       <c r="I147" t="n">
-        <v>0.2044221484230257</v>
+        <v>0.5547191453775073</v>
       </c>
       <c r="J147" t="n">
-        <v>0.1924214877278704</v>
+        <v>0.5101970061718677</v>
       </c>
       <c r="K147" t="n">
-        <v>0.1811253292514385</v>
+        <v>0.4692482444059004</v>
       </c>
       <c r="L147" t="n">
-        <v>0.1603814715722372</v>
+        <v>0.4125421905266581</v>
       </c>
       <c r="M147" t="n">
-        <v>0.1420133590921936</v>
+        <v>0.3626887494912351</v>
       </c>
       <c r="N147" t="n">
-        <v>0.1257489033049841</v>
+        <v>0.3188598209545205</v>
       </c>
       <c r="O147" t="n">
-        <v>0.1113471773605521</v>
+        <v>0.2803273759160427</v>
       </c>
       <c r="P147" t="n">
-        <v>0.0985948471939543</v>
+        <v>0.2464513636516868</v>
       </c>
       <c r="Q147" t="n">
-        <v>0.0868624828170327</v>
+        <v>0.2224973810844635</v>
       </c>
       <c r="R147" t="n">
-        <v>0.07652621953251483</v>
+        <v>0.2008716196815662</v>
       </c>
       <c r="S147" t="n">
-        <v>0.06741992729213483</v>
+        <v>0.1813477866428391</v>
       </c>
       <c r="T147" t="n">
-        <v>0.05939724481157018</v>
+        <v>0.1637215838274773</v>
       </c>
       <c r="U147" t="n">
-        <v>0.05232922717223367</v>
+        <v>0.1478085699704135</v>
       </c>
       <c r="V147" t="n">
-        <v>0.04716108015564285</v>
+        <v>0.1333651363457984</v>
       </c>
       <c r="W147" t="n">
-        <v>0.04250335045320775</v>
+        <v>0.1203330740301028</v>
       </c>
       <c r="X147" t="n">
-        <v>0.0383056281532611</v>
+        <v>0.1085744678278536</v>
       </c>
       <c r="Y147" t="n">
-        <v>0.03452248193542515</v>
+        <v>0.09796487922474752</v>
       </c>
       <c r="Z147" t="n">
-        <v>0.03111296737422889</v>
+        <v>0.08839202948464581</v>
       </c>
       <c r="AA147" t="n">
-        <v>0.0272434683873872</v>
+        <v>0.08125937669199293</v>
       </c>
       <c r="AB147" t="n">
-        <v>0.02346381675930415</v>
+        <v>0.07470228185583402</v>
       </c>
       <c r="AC147" t="n">
-        <v>0.01977239538807939</v>
+        <v>0.06867430125166528</v>
       </c>
       <c r="AD147" t="n">
-        <v>0.01616761326553171</v>
+        <v>0.06313273885670678</v>
       </c>
       <c r="AE147" t="n">
-        <v>0.01264790508108799</v>
+        <v>0.05803834393513373</v>
       </c>
       <c r="AF147" t="n">
-        <v>0.01000189914383351</v>
+        <v>0.05278345679416995</v>
       </c>
       <c r="AG147" t="n">
-        <v>0.007415110386022627</v>
+        <v>0.04800435577996279</v>
       </c>
       <c r="AH147" t="n">
-        <v>0.004886526381635559</v>
+        <v>0.04365796243386195</v>
       </c>
       <c r="AI147" t="n">
-        <v>0.002415150163182019</v>
+        <v>0.03970509869173333</v>
       </c>
       <c r="AJ147" t="n">
-        <v>8.347371196180169e-19</v>
+        <v>0.03611013373582281</v>
       </c>
     </row>
     <row r="148">
@@ -24408,100 +24408,100 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>0.2232643935843875</v>
+        <v>0.835583733802869</v>
       </c>
       <c r="F149" t="n">
-        <v>0.2060354417076212</v>
+        <v>0.7645196348684461</v>
       </c>
       <c r="G149" t="n">
-        <v>0.1901360201603731</v>
+        <v>0.6994993421416639</v>
       </c>
       <c r="H149" t="n">
-        <v>0.1754635312390943</v>
+        <v>0.6400088465233679</v>
       </c>
       <c r="I149" t="n">
-        <v>0.1619232945389542</v>
+        <v>0.5855778539749028</v>
       </c>
       <c r="J149" t="n">
-        <v>0.149427935988713</v>
+        <v>0.5357760676724219</v>
       </c>
       <c r="K149" t="n">
-        <v>0.1378968240327845</v>
+        <v>0.4902097863537485</v>
       </c>
       <c r="L149" t="n">
-        <v>0.124585039116332</v>
+        <v>0.4381469978127851</v>
       </c>
       <c r="M149" t="n">
-        <v>0.1125582991521823</v>
+        <v>0.3916135439079627</v>
       </c>
       <c r="N149" t="n">
-        <v>0.1016925531178912</v>
+        <v>0.3500221809979928</v>
       </c>
       <c r="O149" t="n">
-        <v>0.09187572518000885</v>
+        <v>0.3128480337222079</v>
       </c>
       <c r="P149" t="n">
-        <v>0.08300655867659033</v>
+        <v>0.2796219711699156</v>
       </c>
       <c r="Q149" t="n">
-        <v>0.07651487803778154</v>
+        <v>0.2590240908194688</v>
       </c>
       <c r="R149" t="n">
-        <v>0.07053089122688432</v>
+        <v>0.239943518544479</v>
       </c>
       <c r="S149" t="n">
-        <v>0.06501489311401927</v>
+        <v>0.2222684844076188</v>
       </c>
       <c r="T149" t="n">
-        <v>0.05993028378203968</v>
+        <v>0.2058954518152649</v>
       </c>
       <c r="U149" t="n">
-        <v>0.05524332567765673</v>
+        <v>0.1907285110221364</v>
       </c>
       <c r="V149" t="n">
-        <v>0.04819425106284949</v>
+        <v>0.1738458128631536</v>
       </c>
       <c r="W149" t="n">
-        <v>0.04204464171946808</v>
+        <v>0.1584575189523865</v>
       </c>
       <c r="X149" t="n">
-        <v>0.03667972545134344</v>
+        <v>0.1444313492457298</v>
       </c>
       <c r="Y149" t="n">
-        <v>0.03199937504909134</v>
+        <v>0.1316467327196391</v>
       </c>
       <c r="Z149" t="n">
-        <v>0.0279162395828376</v>
+        <v>0.1199937709248292</v>
       </c>
       <c r="AA149" t="n">
-        <v>0.02401272965577615</v>
+        <v>0.1129850550529576</v>
       </c>
       <c r="AB149" t="n">
-        <v>0.02065504502532931</v>
+        <v>0.1063857112492695</v>
       </c>
       <c r="AC149" t="n">
-        <v>0.01776686328935358</v>
+        <v>0.1001718285016375</v>
       </c>
       <c r="AD149" t="n">
-        <v>0.01528253415838522</v>
+        <v>0.09432089241618317</v>
       </c>
       <c r="AE149" t="n">
-        <v>0.01314558718094964</v>
+        <v>0.08881170364220486</v>
       </c>
       <c r="AF149" t="n">
-        <v>0.0102632997329713</v>
+        <v>0.08276702264108957</v>
       </c>
       <c r="AG149" t="n">
-        <v>0.007512168339187448</v>
+        <v>0.07713375327725627</v>
       </c>
       <c r="AH149" t="n">
-        <v>0.004887548590028592</v>
+        <v>0.07188389414992639</v>
       </c>
       <c r="AI149" t="n">
-        <v>0.002384943681501119</v>
+        <v>0.06699134968298573</v>
       </c>
       <c r="AJ149" t="n">
-        <v>-6.505612540664718e-19</v>
+        <v>0.06243180041120056</v>
       </c>
     </row>
     <row r="150">
@@ -24514,100 +24514,100 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>0.4172728350519271</v>
+        <v>1.029592175270409</v>
       </c>
       <c r="F150" t="n">
-        <v>0.3803760611783639</v>
+        <v>0.9388074778699153</v>
       </c>
       <c r="G150" t="n">
-        <v>0.3467418335525272</v>
+        <v>0.8560277570806073</v>
       </c>
       <c r="H150" t="n">
-        <v>0.3160816660304785</v>
+        <v>0.7805471709227187</v>
       </c>
       <c r="I150" t="n">
-        <v>0.288132581456942</v>
+        <v>0.7117221153123072</v>
       </c>
       <c r="J150" t="n">
-        <v>0.2626548560682287</v>
+        <v>0.6489657362101671</v>
       </c>
       <c r="K150" t="n">
-        <v>0.2394299633432166</v>
+        <v>0.5917429256641807</v>
       </c>
       <c r="L150" t="n">
-        <v>0.2113815413552753</v>
+        <v>0.5249182810834528</v>
       </c>
       <c r="M150" t="n">
-        <v>0.1866188984946769</v>
+        <v>0.4656400437847867</v>
       </c>
       <c r="N150" t="n">
-        <v>0.1647571166908676</v>
+        <v>0.4130560092675213</v>
       </c>
       <c r="O150" t="n">
-        <v>0.1454563697420089</v>
+        <v>0.3664102112121331</v>
       </c>
       <c r="P150" t="n">
-        <v>0.1284166409528867</v>
+        <v>0.3250320534462119</v>
       </c>
       <c r="Q150" t="n">
-        <v>0.1143982279663769</v>
+        <v>0.2971376765455484</v>
       </c>
       <c r="R150" t="n">
-        <v>0.1019101143336125</v>
+        <v>0.2716372058902117</v>
       </c>
       <c r="S150" t="n">
-        <v>0.09078524718531866</v>
+        <v>0.2483251955176758</v>
       </c>
       <c r="T150" t="n">
-        <v>0.08087480973202098</v>
+        <v>0.2270138309176078</v>
       </c>
       <c r="U150" t="n">
-        <v>0.07204623054932134</v>
+        <v>0.207531415893801</v>
       </c>
       <c r="V150" t="n">
-        <v>0.0624263277377939</v>
+        <v>0.1881954848623017</v>
       </c>
       <c r="W150" t="n">
-        <v>0.05409091308612766</v>
+        <v>0.1706611038623707</v>
       </c>
       <c r="X150" t="n">
-        <v>0.04686847656296902</v>
+        <v>0.1547604204895411</v>
       </c>
       <c r="Y150" t="n">
-        <v>0.04061040884697023</v>
+        <v>0.1403412213330968</v>
       </c>
       <c r="Z150" t="n">
-        <v>0.03518794353177509</v>
+        <v>0.1272654748737667</v>
       </c>
       <c r="AA150" t="n">
-        <v>0.03079939620932258</v>
+        <v>0.1189996753765431</v>
       </c>
       <c r="AB150" t="n">
-        <v>0.02662474340430953</v>
+        <v>0.1112707335101583</v>
       </c>
       <c r="AC150" t="n">
-        <v>0.02265556337266317</v>
+        <v>0.1040437807642055</v>
       </c>
       <c r="AD150" t="n">
-        <v>0.01888373516355893</v>
+        <v>0.09728621331252195</v>
       </c>
       <c r="AE150" t="n">
-        <v>0.01530142846234934</v>
+        <v>0.09096754492360457</v>
       </c>
       <c r="AF150" t="n">
-        <v>0.01194645355053396</v>
+        <v>0.08437044718739263</v>
       </c>
       <c r="AG150" t="n">
-        <v>0.008744143936436823</v>
+        <v>0.07825178050675863</v>
       </c>
       <c r="AH150" t="n">
-        <v>0.005689093539690506</v>
+        <v>0.07257684837058601</v>
       </c>
       <c r="AI150" t="n">
-        <v>0.002776068092424701</v>
+        <v>0.06731347050885425</v>
       </c>
       <c r="AJ150" t="n">
-        <v>0</v>
+        <v>0.06243180041120055</v>
       </c>
     </row>
     <row r="151">
@@ -24734,100 +24734,100 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>0.1670648452299242</v>
+        <v>0.8722525956829762</v>
       </c>
       <c r="F152" t="n">
-        <v>0.1565303719856432</v>
+        <v>0.7972964329975255</v>
       </c>
       <c r="G152" t="n">
-        <v>0.1466601625269705</v>
+        <v>0.7287815538947606</v>
       </c>
       <c r="H152" t="n">
-        <v>0.1374123309079607</v>
+        <v>0.6661544330512642</v>
       </c>
       <c r="I152" t="n">
-        <v>0.1287476323509904</v>
+        <v>0.6089091117939195</v>
       </c>
       <c r="J152" t="n">
-        <v>0.1206292967047363</v>
+        <v>0.5565831105069403</v>
       </c>
       <c r="K152" t="n">
-        <v>0.1130228724036598</v>
+        <v>0.5087536923021531</v>
       </c>
       <c r="L152" t="n">
-        <v>0.0984590017893211</v>
+        <v>0.4452844867711186</v>
       </c>
       <c r="M152" t="n">
-        <v>0.08577179846152648</v>
+        <v>0.3897333368958814</v>
       </c>
       <c r="N152" t="n">
-        <v>0.07471943933645117</v>
+        <v>0.3411124312670538</v>
       </c>
       <c r="O152" t="n">
-        <v>0.06509126210356773</v>
+        <v>0.2985571921860148</v>
       </c>
       <c r="P152" t="n">
-        <v>0.05670374991917846</v>
+        <v>0.2613109017308516</v>
       </c>
       <c r="Q152" t="n">
-        <v>0.05319244156673527</v>
+        <v>0.2409315902460146</v>
       </c>
       <c r="R152" t="n">
-        <v>0.04989856656505831</v>
+        <v>0.2221416358597337</v>
       </c>
       <c r="S152" t="n">
-        <v>0.04680866062753984</v>
+        <v>0.2048170865931301</v>
       </c>
       <c r="T152" t="n">
-        <v>0.0439100932265756</v>
+        <v>0.1888436573276437</v>
       </c>
       <c r="U152" t="n">
-        <v>0.04119101596408777</v>
+        <v>0.1741159758986468</v>
       </c>
       <c r="V152" t="n">
-        <v>0.03553850316783902</v>
+        <v>0.1544683858879683</v>
       </c>
       <c r="W152" t="n">
-        <v>0.0300908747355031</v>
+        <v>0.1370378686716462</v>
       </c>
       <c r="X152" t="n">
-        <v>0.02484228760800545</v>
+        <v>0.1215742453843437</v>
       </c>
       <c r="Y152" t="n">
-        <v>0.01978704873609474</v>
+        <v>0.1078555678371459</v>
       </c>
       <c r="Z152" t="n">
-        <v>0.0149196114510454</v>
+        <v>0.09568493291237191</v>
       </c>
       <c r="AA152" t="n">
-        <v>0.01314079950379817</v>
+        <v>0.09012495727270421</v>
       </c>
       <c r="AB152" t="n">
-        <v>0.01142884693708117</v>
+        <v>0.08488805579082484</v>
       </c>
       <c r="AC152" t="n">
-        <v>0.009781755981858729</v>
+        <v>0.07995545555868618</v>
       </c>
       <c r="AD152" t="n">
-        <v>0.008197582764025463</v>
+        <v>0.07530947450781429</v>
       </c>
       <c r="AE152" t="n">
-        <v>0.006674435932545018</v>
+        <v>0.07093345802376572</v>
       </c>
       <c r="AF152" t="n">
-        <v>0.00523997653898446</v>
+        <v>0.0664908085491137</v>
       </c>
       <c r="AG152" t="n">
-        <v>0.003856695870061785</v>
+        <v>0.06232640765988964</v>
       </c>
       <c r="AH152" t="n">
-        <v>0.002523183991546703</v>
+        <v>0.05842282830592126</v>
       </c>
       <c r="AI152" t="n">
-        <v>0.001238065756873298</v>
+        <v>0.0547637349145625</v>
       </c>
       <c r="AJ152" t="n">
-        <v>3.480431220361742e-19</v>
+        <v>0.05133381503011745</v>
       </c>
     </row>
     <row r="153">
@@ -24840,100 +24840,100 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>0.275131903809969</v>
+        <v>0.980319654263021</v>
       </c>
       <c r="F153" t="n">
-        <v>0.2530624529023717</v>
+        <v>0.8935888480552218</v>
       </c>
       <c r="G153" t="n">
-        <v>0.232763282564269</v>
+        <v>0.8145312867045909</v>
       </c>
       <c r="H153" t="n">
-        <v>0.2140923913789581</v>
+        <v>0.7424681031601637</v>
       </c>
       <c r="I153" t="n">
-        <v>0.196919168441892</v>
+        <v>0.6767804910729951</v>
       </c>
       <c r="J153" t="n">
-        <v>0.1811234796812934</v>
+        <v>0.6169043911078275</v>
       </c>
       <c r="K153" t="n">
-        <v>0.1665948274687153</v>
+        <v>0.5623256473672087</v>
       </c>
       <c r="L153" t="n">
-        <v>0.1451831293293015</v>
+        <v>0.486173915109421</v>
       </c>
       <c r="M153" t="n">
-        <v>0.1245435950977603</v>
+        <v>0.4203348661749229</v>
       </c>
       <c r="N153" t="n">
-        <v>0.1046542432917499</v>
+        <v>0.363411927771825</v>
       </c>
       <c r="O153" t="n">
-        <v>0.08549365626489966</v>
+        <v>0.3141976549522633</v>
       </c>
       <c r="P153" t="n">
-        <v>0.06704096657228022</v>
+        <v>0.2716481183839535</v>
       </c>
       <c r="Q153" t="n">
-        <v>0.06318345866107282</v>
+        <v>0.2509505753006293</v>
       </c>
       <c r="R153" t="n">
-        <v>0.0595479100688586</v>
+        <v>0.2318300292980673</v>
       </c>
       <c r="S153" t="n">
-        <v>0.05612154935344692</v>
+        <v>0.2141663250620489</v>
       </c>
       <c r="T153" t="n">
-        <v>0.05289233993584805</v>
+        <v>0.1978484622094018</v>
       </c>
       <c r="U153" t="n">
-        <v>0.04984893781656584</v>
+        <v>0.1827738977511249</v>
       </c>
       <c r="V153" t="n">
-        <v>0.04293810526668444</v>
+        <v>0.1615159431670989</v>
       </c>
       <c r="W153" t="n">
-        <v>0.0362779616746017</v>
+        <v>0.1427304457482194</v>
       </c>
       <c r="X153" t="n">
-        <v>0.0298613556430091</v>
+        <v>0.1261298404604506</v>
       </c>
       <c r="Y153" t="n">
-        <v>0.02368131940090795</v>
+        <v>0.1114600082076546</v>
       </c>
       <c r="Z153" t="n">
-        <v>0.01773106436059877</v>
+        <v>0.09849638582192528</v>
       </c>
       <c r="AA153" t="n">
-        <v>0.01519881700022838</v>
+        <v>0.09263208253840918</v>
       </c>
       <c r="AB153" t="n">
-        <v>0.01302821046207236</v>
+        <v>0.08711692965989606</v>
       </c>
       <c r="AC153" t="n">
-        <v>0.01116759730981044</v>
+        <v>0.08193013937930642</v>
       </c>
       <c r="AD153" t="n">
-        <v>0.009572706093224054</v>
+        <v>0.07705216155939287</v>
       </c>
       <c r="AE153" t="n">
-        <v>0.008205587952813134</v>
+        <v>0.07246461004403384</v>
       </c>
       <c r="AF153" t="n">
-        <v>0.006697616924050023</v>
+        <v>0.06794600980451411</v>
       </c>
       <c r="AG153" t="n">
-        <v>0.005243033860051793</v>
+        <v>0.06370917121543562</v>
       </c>
       <c r="AH153" t="n">
-        <v>0.003840371994190595</v>
+        <v>0.05973652475892754</v>
       </c>
       <c r="AI153" t="n">
-        <v>0.002488200698867191</v>
+        <v>0.05601159648125181</v>
       </c>
       <c r="AJ153" t="n">
-        <v>0.001185124647733771</v>
+        <v>0.05251893967785121</v>
       </c>
     </row>
     <row r="154">

</xml_diff>

<commit_message>
Post-linting cleanups and releng updates
First attempt to copy patterns from os-climate/ITR into os-climate/itr-data-pipeline bring the latter up to releng scratch with the former.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/notebooks/benchmark_OECM_PC.xlsx
+++ b/notebooks/benchmark_OECM_PC.xlsx
@@ -8533,29 +8533,29 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
     <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
     <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A67"/>
     <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A56:A58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -31283,167 +31283,167 @@
     </row>
   </sheetData>
   <mergeCells count="161">
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="C95:C97"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="C131:C133"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C194:C196"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="A29:A37"/>
+    <mergeCell ref="A38:A46"/>
+    <mergeCell ref="A47:A55"/>
+    <mergeCell ref="A56:A64"/>
+    <mergeCell ref="A65:A73"/>
+    <mergeCell ref="A74:A82"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A92:A100"/>
     <mergeCell ref="A101:A109"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="C179:C181"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="A200:A208"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C155:C157"/>
-    <mergeCell ref="C107:C109"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="C101:C103"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="B152:B154"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="C206:C208"/>
-    <mergeCell ref="B167:B169"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B176:B178"/>
-    <mergeCell ref="C143:C145"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B191:B193"/>
-    <mergeCell ref="B107:B109"/>
-    <mergeCell ref="B128:B130"/>
-    <mergeCell ref="C122:C124"/>
-    <mergeCell ref="A164:A172"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="B197:B199"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B188:B190"/>
-    <mergeCell ref="B206:B208"/>
-    <mergeCell ref="C125:C127"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="C170:C172"/>
-    <mergeCell ref="B203:B205"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="B131:B133"/>
-    <mergeCell ref="B140:B142"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="B149:B151"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="A182:A190"/>
-    <mergeCell ref="B182:B184"/>
-    <mergeCell ref="C137:C139"/>
-    <mergeCell ref="A191:A199"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C197:C199"/>
-    <mergeCell ref="C146:C148"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C173:C175"/>
-    <mergeCell ref="C188:C190"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C182:C184"/>
-    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="A110:A118"/>
+    <mergeCell ref="A119:A127"/>
+    <mergeCell ref="A128:A136"/>
     <mergeCell ref="A137:A145"/>
     <mergeCell ref="A146:A154"/>
+    <mergeCell ref="A155:A163"/>
+    <mergeCell ref="A164:A172"/>
+    <mergeCell ref="A173:A181"/>
+    <mergeCell ref="A182:A190"/>
+    <mergeCell ref="A191:A199"/>
+    <mergeCell ref="A200:A208"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="B107:B109"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="B140:B142"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="B146:B148"/>
+    <mergeCell ref="B149:B151"/>
+    <mergeCell ref="B152:B154"/>
+    <mergeCell ref="B155:B157"/>
+    <mergeCell ref="B158:B160"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="B167:B169"/>
+    <mergeCell ref="B170:B172"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="B176:B178"/>
+    <mergeCell ref="B179:B181"/>
+    <mergeCell ref="B182:B184"/>
+    <mergeCell ref="B185:B187"/>
+    <mergeCell ref="B188:B190"/>
+    <mergeCell ref="B191:B193"/>
+    <mergeCell ref="B194:B196"/>
+    <mergeCell ref="B197:B199"/>
+    <mergeCell ref="B200:B202"/>
+    <mergeCell ref="B203:B205"/>
+    <mergeCell ref="B206:B208"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="C107:C109"/>
     <mergeCell ref="C110:C112"/>
-    <mergeCell ref="A65:A73"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="C116:C118"/>
     <mergeCell ref="C119:C121"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="B158:B160"/>
-    <mergeCell ref="A74:A82"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="A56:A64"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="C128:C130"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="C134:C136"/>
+    <mergeCell ref="C137:C139"/>
+    <mergeCell ref="C140:C142"/>
+    <mergeCell ref="C143:C145"/>
+    <mergeCell ref="C146:C148"/>
+    <mergeCell ref="C149:C151"/>
+    <mergeCell ref="C152:C154"/>
+    <mergeCell ref="C155:C157"/>
     <mergeCell ref="C158:C160"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B185:B187"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B194:B196"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A155:A163"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="C128:C130"/>
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="A92:A100"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="C164:C166"/>
+    <mergeCell ref="C167:C169"/>
+    <mergeCell ref="C170:C172"/>
+    <mergeCell ref="C173:C175"/>
+    <mergeCell ref="C176:C178"/>
+    <mergeCell ref="C179:C181"/>
+    <mergeCell ref="C182:C184"/>
     <mergeCell ref="C185:C187"/>
+    <mergeCell ref="C188:C190"/>
+    <mergeCell ref="C191:C193"/>
+    <mergeCell ref="C194:C196"/>
+    <mergeCell ref="C197:C199"/>
     <mergeCell ref="C200:C202"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B155:B157"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="C176:C178"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="B179:B181"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C134:C136"/>
-    <mergeCell ref="A110:A118"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C164:C166"/>
-    <mergeCell ref="A119:A127"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="A128:A136"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="B143:B145"/>
     <mergeCell ref="C203:C205"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C140:C142"/>
-    <mergeCell ref="C149:C151"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="B122:B124"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C191:C193"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="B200:B202"/>
-    <mergeCell ref="A38:A46"/>
-    <mergeCell ref="B161:B163"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B170:B172"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C152:C154"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="C167:C169"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="A173:A181"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="C206:C208"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>